<commit_message>
Worked on feature extraction, changed name "previous_tuple" to "tuple_minus1", added some global lists for feature extraction
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281D742A-B46D-4FAC-A4D7-9F3A551BC235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FED6EA2-6457-4240-B931-021F686F3CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="171">
   <si>
     <t/>
   </si>
@@ -543,6 +543,21 @@
   </si>
   <si>
     <t>"superlatives_213"</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So far, the identification of demonstrative pronouns is probably still too imprecise. We would need to re-use the extraction for feature 10. </t>
+  </si>
+  <si>
+    <t>Biber says that here he "excludes demonstrative pronouns (no. 10) and that as relative, complementizer, or subordinator." Instead, we look at all words tagged as determiners and then count the ones that are "that, this, these, those"</t>
+  </si>
+  <si>
+    <t>The tag we are using to find prepositions (IN) does probably not overlap 100% with what Biber understood as prepositions</t>
+  </si>
+  <si>
+    <t>Here, Biber also counts "any ADJ not identified as predicative - no. 41)", so far we do not do that</t>
   </si>
 </sst>
 </file>
@@ -930,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1255,7 +1270,9 @@
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -1329,7 +1346,9 @@
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
@@ -1419,7 +1438,9 @@
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -1509,7 +1530,9 @@
       <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
@@ -1536,7 +1559,9 @@
       <c r="B65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
@@ -1545,7 +1570,9 @@
       <c r="B66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="1"/>
+      <c r="C66" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">

</xml_diff>

<commit_message>
Worked on feature extraction
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FED6EA2-6457-4240-B931-021F686F3CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C248683F-1268-492E-8405-4262B0A0E6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
   <si>
     <t/>
   </si>
@@ -558,6 +558,9 @@
   </si>
   <si>
     <t>Here, Biber also counts "any ADJ not identified as predicative - no. 41)", so far we do not do that</t>
+  </si>
+  <si>
+    <t>we use the EX tag for this, not the code by Biber</t>
   </si>
 </sst>
 </file>
@@ -945,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,7 +1156,9 @@
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">

</xml_diff>

<commit_message>
Start testing precision & recall for several features, did not manage to fix problem with "list index out of range", but managed to set up my own test script, yeah :)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C248683F-1268-492E-8405-4262B0A0E6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C53D9-21CE-4AD7-BEA2-39F0C58C5DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="176">
   <si>
     <t/>
   </si>
@@ -561,6 +561,18 @@
   </si>
   <si>
     <t>we use the EX tag for this, not the code by Biber</t>
+  </si>
+  <si>
+    <t>the count this gives seems too high or too low in many cases</t>
+  </si>
+  <si>
+    <t>very imprecise, also counts "everything", "something"</t>
+  </si>
+  <si>
+    <t>seems to work fairly well, but also catches stuff like "cities"</t>
+  </si>
+  <si>
+    <t>appears to be workgin well</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,10 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -628,22 +643,24 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" headers="0" connectionId="1" xr16:uid="{355E3EDC-A711-4EA7-BF39-4E4F5FF40C4F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh headersInLastRefresh="0" nextId="4" unboundColumnsRight="1">
-    <queryTableFields count="3">
+  <queryTableRefresh headersInLastRefresh="0" nextId="5" unboundColumnsRight="2">
+    <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" dataBound="0" tableColumnId="3"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40D99BE-96FE-4629-88D4-1F8802B80194}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:C81" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD1E9984-ECA3-410E-BA89-2B6D8BFFC517}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D21A4EB7-50A6-4AF1-85B1-4F1BD5983C4D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{CA1DE6FC-A106-455D-85F9-B24344C1C7FD}" uniqueName="3" name="Spalte1" queryTableFieldId="3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40D99BE-96FE-4629-88D4-1F8802B80194}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D81" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CD1E9984-ECA3-410E-BA89-2B6D8BFFC517}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D21A4EB7-50A6-4AF1-85B1-4F1BD5983C4D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{CA1DE6FC-A106-455D-85F9-B24344C1C7FD}" uniqueName="3" name="Spalte1" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{25B9C599-A2D1-4D0D-9C03-D14F3D1CE5F2}" uniqueName="4" name="Spalte2" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -948,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,6 +1003,7 @@
       <c r="C2" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -995,6 +1013,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1004,6 +1023,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1013,6 +1033,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1022,6 +1043,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1031,6 +1053,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1040,6 +1063,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1049,6 +1073,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1058,6 +1083,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1067,6 +1093,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -1076,6 +1103,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1085,6 +1113,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -1094,6 +1123,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -1103,6 +1133,9 @@
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -1112,8 +1145,11 @@
         <v>15</v>
       </c>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -1121,8 +1157,11 @@
         <v>16</v>
       </c>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>102</v>
       </c>
@@ -1130,8 +1169,9 @@
         <v>17</v>
       </c>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -1139,8 +1179,9 @@
         <v>18</v>
       </c>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>104</v>
       </c>
@@ -1148,8 +1189,9 @@
         <v>19</v>
       </c>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>105</v>
       </c>
@@ -1159,8 +1201,11 @@
       <c r="C21" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>106</v>
       </c>
@@ -1168,8 +1213,9 @@
         <v>21</v>
       </c>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>107</v>
       </c>
@@ -1177,8 +1223,9 @@
         <v>22</v>
       </c>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>108</v>
       </c>
@@ -1186,8 +1233,9 @@
         <v>23</v>
       </c>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
@@ -1195,8 +1243,9 @@
         <v>24</v>
       </c>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>110</v>
       </c>
@@ -1204,8 +1253,9 @@
         <v>25</v>
       </c>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>111</v>
       </c>
@@ -1213,8 +1263,9 @@
         <v>26</v>
       </c>
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
@@ -1222,8 +1273,9 @@
         <v>27</v>
       </c>
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1231,8 +1283,9 @@
         <v>28</v>
       </c>
       <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>114</v>
       </c>
@@ -1240,8 +1293,9 @@
         <v>29</v>
       </c>
       <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -1249,8 +1303,9 @@
         <v>30</v>
       </c>
       <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>116</v>
       </c>
@@ -1258,8 +1313,9 @@
         <v>31</v>
       </c>
       <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
@@ -1267,8 +1323,9 @@
         <v>32</v>
       </c>
       <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -1278,8 +1335,9 @@
       <c r="C34" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>119</v>
       </c>
@@ -1287,8 +1345,9 @@
         <v>34</v>
       </c>
       <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>120</v>
       </c>
@@ -1296,8 +1355,9 @@
         <v>35</v>
       </c>
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>121</v>
       </c>
@@ -1305,8 +1365,9 @@
         <v>36</v>
       </c>
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>122</v>
       </c>
@@ -1314,8 +1375,9 @@
         <v>37</v>
       </c>
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>123</v>
       </c>
@@ -1323,8 +1385,9 @@
         <v>38</v>
       </c>
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>124</v>
       </c>
@@ -1334,8 +1397,9 @@
       <c r="C40" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>125</v>
       </c>
@@ -1343,8 +1407,9 @@
         <v>40</v>
       </c>
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>126</v>
       </c>
@@ -1354,8 +1419,9 @@
       <c r="C42" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -1363,8 +1429,9 @@
         <v>42</v>
       </c>
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>128</v>
       </c>
@@ -1372,8 +1439,9 @@
         <v>43</v>
       </c>
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
@@ -1381,8 +1449,9 @@
         <v>44</v>
       </c>
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
@@ -1390,8 +1459,9 @@
         <v>45</v>
       </c>
       <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>131</v>
       </c>
@@ -1399,8 +1469,9 @@
         <v>46</v>
       </c>
       <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>132</v>
       </c>
@@ -1408,8 +1479,9 @@
         <v>47</v>
       </c>
       <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>133</v>
       </c>
@@ -1417,8 +1489,9 @@
         <v>48</v>
       </c>
       <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>134</v>
       </c>
@@ -1426,8 +1499,9 @@
         <v>49</v>
       </c>
       <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>135</v>
       </c>
@@ -1435,8 +1509,9 @@
         <v>50</v>
       </c>
       <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>136</v>
       </c>
@@ -1446,8 +1521,9 @@
       <c r="C52" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>137</v>
       </c>
@@ -1455,8 +1531,9 @@
         <v>52</v>
       </c>
       <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>138</v>
       </c>
@@ -1464,8 +1541,9 @@
         <v>53</v>
       </c>
       <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>139</v>
       </c>
@@ -1473,8 +1551,9 @@
         <v>54</v>
       </c>
       <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
@@ -1482,8 +1561,9 @@
         <v>55</v>
       </c>
       <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>141</v>
       </c>
@@ -1491,8 +1571,9 @@
         <v>56</v>
       </c>
       <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>142</v>
       </c>
@@ -1500,8 +1581,9 @@
         <v>57</v>
       </c>
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -1509,8 +1591,9 @@
         <v>58</v>
       </c>
       <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -1518,8 +1601,9 @@
         <v>59</v>
       </c>
       <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -1527,8 +1611,9 @@
         <v>60</v>
       </c>
       <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
@@ -1538,8 +1623,9 @@
       <c r="C62" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -1547,8 +1633,9 @@
         <v>62</v>
       </c>
       <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -1556,8 +1643,9 @@
         <v>63</v>
       </c>
       <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>149</v>
       </c>
@@ -1567,8 +1655,9 @@
       <c r="C65" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>150</v>
       </c>
@@ -1578,8 +1667,9 @@
       <c r="C66" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>151</v>
       </c>
@@ -1587,8 +1677,9 @@
         <v>66</v>
       </c>
       <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>152</v>
       </c>
@@ -1596,8 +1687,9 @@
         <v>67</v>
       </c>
       <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>153</v>
       </c>
@@ -1605,8 +1697,9 @@
         <v>68</v>
       </c>
       <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>154</v>
       </c>
@@ -1614,8 +1707,9 @@
         <v>69</v>
       </c>
       <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>155</v>
       </c>
@@ -1623,8 +1717,9 @@
         <v>70</v>
       </c>
       <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>156</v>
       </c>
@@ -1632,8 +1727,9 @@
         <v>71</v>
       </c>
       <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>157</v>
       </c>
@@ -1641,8 +1737,9 @@
         <v>72</v>
       </c>
       <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>158</v>
       </c>
@@ -1650,8 +1747,9 @@
         <v>0</v>
       </c>
       <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>159</v>
       </c>
@@ -1659,8 +1757,9 @@
         <v>0</v>
       </c>
       <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>160</v>
       </c>
@@ -1668,8 +1767,9 @@
         <v>73</v>
       </c>
       <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>161</v>
       </c>
@@ -1677,8 +1777,9 @@
         <v>74</v>
       </c>
       <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>162</v>
       </c>
@@ -1686,8 +1787,9 @@
         <v>75</v>
       </c>
       <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>163</v>
       </c>
@@ -1695,8 +1797,9 @@
         <v>76</v>
       </c>
       <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>164</v>
       </c>
@@ -1704,8 +1807,9 @@
         <v>77</v>
       </c>
       <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>165</v>
       </c>
@@ -1713,6 +1817,7 @@
         <v>78</v>
       </c>
       <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tested precision&recall for several features, solved list index issue :) yeah!
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C53D9-21CE-4AD7-BEA2-39F0C58C5DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B8D949-0B6B-494D-9A2D-A1EDA5DC6C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="7760" yWindow="240" windowWidth="11000" windowHeight="9620" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="180">
   <si>
     <t/>
   </si>
@@ -573,6 +573,18 @@
   </si>
   <si>
     <t>appears to be workgin well</t>
+  </si>
+  <si>
+    <t>seems to work well</t>
+  </si>
+  <si>
+    <t>appears to be 100% accurate</t>
+  </si>
+  <si>
+    <t>for some reason this does not catch "i"</t>
+  </si>
+  <si>
+    <t>doesn't work well, but I don't see why</t>
   </si>
 </sst>
 </file>
@@ -965,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1053,7 +1065,9 @@
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1063,7 +1077,9 @@
         <v>7</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1073,7 +1089,9 @@
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1083,7 +1101,9 @@
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1355,7 +1375,9 @@
         <v>35</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
@@ -1521,7 +1543,9 @@
       <c r="C52" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -1677,7 +1701,9 @@
         <v>66</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">

</xml_diff>

<commit_message>
Tested precision & recall, fixed tuple_plus2-definition
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B8D949-0B6B-494D-9A2D-A1EDA5DC6C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962200A5-F356-4667-BE1D-1EB3B1A6176E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="240" windowWidth="11000" windowHeight="9620" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="8240" yWindow="0" windowWidth="11000" windowHeight="9620" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="187">
   <si>
     <t/>
   </si>
@@ -585,6 +585,27 @@
   </si>
   <si>
     <t>doesn't work well, but I don't see why</t>
+  </si>
+  <si>
+    <t>for some reason this does not catch "if"</t>
+  </si>
+  <si>
+    <t>does not catch everything it should</t>
+  </si>
+  <si>
+    <t>seems to work fairly well.</t>
+  </si>
+  <si>
+    <t>does not catch "better" and not every "more"</t>
+  </si>
+  <si>
+    <t>does not catch every "most"</t>
+  </si>
+  <si>
+    <t>appears to count too much</t>
+  </si>
+  <si>
+    <t>appears to count too little</t>
   </si>
 </sst>
 </file>
@@ -977,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1066,9 @@
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1055,7 +1078,9 @@
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1397,7 +1422,9 @@
         <v>37</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
@@ -1429,7 +1456,9 @@
         <v>40</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
@@ -1441,7 +1470,9 @@
       <c r="C42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
@@ -1491,7 +1522,9 @@
         <v>46</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
@@ -1511,7 +1544,9 @@
         <v>48</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
@@ -1713,7 +1748,9 @@
         <v>67</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
@@ -1833,7 +1870,9 @@
         <v>77</v>
       </c>
       <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
+      <c r="D80" s="1" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
@@ -1843,7 +1882,9 @@
         <v>78</v>
       </c>
       <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Worked on adverb-function, added some potential additional items that Biber doesn't have
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962200A5-F356-4667-BE1D-1EB3B1A6176E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043CE848-8106-4E2E-9C56-EC8755F5C44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="0" windowWidth="11000" windowHeight="9620" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
   <si>
     <t/>
   </si>
@@ -584,15 +584,9 @@
     <t>for some reason this does not catch "i"</t>
   </si>
   <si>
-    <t>doesn't work well, but I don't see why</t>
-  </si>
-  <si>
     <t>for some reason this does not catch "if"</t>
   </si>
   <si>
-    <t>does not catch everything it should</t>
-  </si>
-  <si>
     <t>seems to work fairly well.</t>
   </si>
   <si>
@@ -606,6 +600,24 @@
   </si>
   <si>
     <t>appears to count too little</t>
+  </si>
+  <si>
+    <t>does not catch everything it should, but the reason seems to be the tagging, not the function</t>
+  </si>
+  <si>
+    <t>there are some words that come to mind that could be added to Biber's list of place adverbials: apart, back, here, out, there (HM)</t>
+  </si>
+  <si>
+    <t>there are some words that come to mind that could be added to Biber's list of place adverbials: then, always (HM)</t>
+  </si>
+  <si>
+    <t>does not catch everything it should, but the reason seems to be the tagging, not the function ("because" tagged as IN)</t>
+  </si>
+  <si>
+    <t>does not catch everything it should, but the reason seems to be the tagging, not the function ("though" tagged as IN)</t>
+  </si>
+  <si>
+    <t>also included "tho" as common shortening of "though"</t>
   </si>
 </sst>
 </file>
@@ -998,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,9 +1077,11 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1077,9 +1091,11 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1399,9 +1415,11 @@
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1411,8 +1429,12 @@
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
@@ -1423,7 +1445,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1457,7 +1479,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1471,7 +1493,7 @@
         <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1523,7 +1545,7 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1545,7 +1567,7 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1871,7 +1893,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1883,7 +1905,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on adverb & particle functions
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043CE848-8106-4E2E-9C56-EC8755F5C44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06D9A3-32B2-4372-B101-C5B0D2FA32E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="191">
   <si>
     <t/>
   </si>
@@ -584,12 +584,6 @@
     <t>for some reason this does not catch "i"</t>
   </si>
   <si>
-    <t>for some reason this does not catch "if"</t>
-  </si>
-  <si>
-    <t>seems to work fairly well.</t>
-  </si>
-  <si>
     <t>does not catch "better" and not every "more"</t>
   </si>
   <si>
@@ -611,13 +605,19 @@
     <t>there are some words that come to mind that could be added to Biber's list of place adverbials: then, always (HM)</t>
   </si>
   <si>
-    <t>does not catch everything it should, but the reason seems to be the tagging, not the function ("because" tagged as IN)</t>
-  </si>
-  <si>
-    <t>does not catch everything it should, but the reason seems to be the tagging, not the function ("though" tagged as IN)</t>
-  </si>
-  <si>
     <t>also included "tho" as common shortening of "though"</t>
+  </si>
+  <si>
+    <t>Here we simply count everything that is tagged as an adverb. Biber counts all adverbs in the dictionary, everything that is longer than five letters and ends in -ly, and excludes everything that is counted as a hedge/amplifier/downtoner/placeadverbial/timeadverbial</t>
+  </si>
+  <si>
+    <t>works well</t>
+  </si>
+  <si>
+    <t>there are some words that come to mind that could be added to Biber's list of place adverbials: a little, a bit, a tad (HM)</t>
+  </si>
+  <si>
+    <t>doens't work well yet. Somehow it counted "family members that are RATHER odd" even though that definitely should not be counted. It did not count "ALTOGETHER, this is nice" even though this should be counted.</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1092,10 +1092,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1418,9 +1418,7 @@
       <c r="C36" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>188</v>
-      </c>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
@@ -1430,11 +1428,9 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
@@ -1444,9 +1440,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
@@ -1479,7 +1473,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1493,7 +1487,7 @@
         <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1503,7 +1497,9 @@
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1534,7 +1530,9 @@
         <v>45</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
@@ -1543,9 +1541,11 @@
       <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="D47" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1588,7 +1588,9 @@
         <v>50</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
@@ -1771,7 +1773,7 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1893,7 +1895,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1905,7 +1907,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on pronoun function. Looks like we don't need the CLAWS-tagset for this.
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06D9A3-32B2-4372-B101-C5B0D2FA32E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F606D59-1C0F-497B-8B14-D97965CEBD52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="191">
   <si>
     <t/>
   </si>
@@ -581,9 +581,6 @@
     <t>appears to be 100% accurate</t>
   </si>
   <si>
-    <t>for some reason this does not catch "i"</t>
-  </si>
-  <si>
     <t>does not catch "better" and not every "more"</t>
   </si>
   <si>
@@ -618,6 +615,9 @@
   </si>
   <si>
     <t>doens't work well yet. Somehow it counted "family members that are RATHER odd" even though that definitely should not be counted. It did not count "ALTOGETHER, this is nice" even though this should be counted.</t>
+  </si>
+  <si>
+    <t>this frequently does not catch "i" because it is tagged as NN or JJ</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1092,10 +1092,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1154,7 +1154,9 @@
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -1428,7 +1430,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D37" s="1"/>
     </row>
@@ -1473,7 +1475,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1487,7 +1489,7 @@
         <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1498,7 +1500,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D43" s="1"/>
     </row>
@@ -1531,7 +1533,7 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1542,10 +1544,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1567,7 +1569,7 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1589,7 +1591,7 @@
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1773,7 +1775,7 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1895,7 +1897,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1907,7 +1909,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second check on analyse_noun function, added some stopwords (precision problems are mainly due to the tagger)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F606D59-1C0F-497B-8B14-D97965CEBD52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FAA80-3E34-43A5-93D3-4B75C2B366D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="192">
   <si>
     <t/>
   </si>
@@ -563,15 +563,6 @@
     <t>we use the EX tag for this, not the code by Biber</t>
   </si>
   <si>
-    <t>the count this gives seems too high or too low in many cases</t>
-  </si>
-  <si>
-    <t>very imprecise, also counts "everything", "something"</t>
-  </si>
-  <si>
-    <t>seems to work fairly well, but also catches stuff like "cities"</t>
-  </si>
-  <si>
     <t>appears to be workgin well</t>
   </si>
   <si>
@@ -618,6 +609,18 @@
   </si>
   <si>
     <t>this frequently does not catch "i" because it is tagged as NN or JJ</t>
+  </si>
+  <si>
+    <t>edited manually by biber, we just use the ing-ending</t>
+  </si>
+  <si>
+    <t>some problems that result from the tagger (e.g. '*' tagged as noun, 'way' in 'this is way better' tagged as noun, 'professional' in 'he is a professional' tagged as adjective)</t>
+  </si>
+  <si>
+    <t>seems to work fairly well</t>
+  </si>
+  <si>
+    <t>added stopword list to avoid counting of "everything", "something". Many gerunds are not counted but that is due to the tagger classifying them as verbs.</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1014,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,10 +1081,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1092,10 +1095,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1107,7 +1110,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1119,7 +1122,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,7 +1134,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1143,7 +1146,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1155,7 +1158,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1197,7 +1200,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1207,9 +1210,11 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1221,7 +1226,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1265,7 +1270,7 @@
         <v>171</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1430,7 +1435,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D37" s="1"/>
     </row>
@@ -1475,7 +1480,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1489,7 +1494,7 @@
         <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1500,7 +1505,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D43" s="1"/>
     </row>
@@ -1533,7 +1538,7 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1544,10 +1549,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1569,7 +1574,7 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1591,7 +1596,7 @@
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1605,7 +1610,7 @@
         <v>168</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1763,7 +1768,7 @@
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1775,7 +1780,7 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1897,7 +1902,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1909,7 +1914,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second check on analyse_modal function (precision problems are mainly due to the tagger)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FAA80-3E34-43A5-93D3-4B75C2B366D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA7FE5-6BF8-4615-84BB-5BEDDAAD9878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="7940" yWindow="5500" windowWidth="11090" windowHeight="4300" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="196">
   <si>
     <t/>
   </si>
@@ -621,6 +621,18 @@
   </si>
   <si>
     <t>added stopword list to avoid counting of "everything", "something". Many gerunds are not counted but that is due to the tagger classifying them as verbs.</t>
+  </si>
+  <si>
+    <t>so far we only use the full forms (can, may, might, could), while Biber also includes the contractions</t>
+  </si>
+  <si>
+    <t>so far we only use the full forms (ought, should, must), while Biber also includes the contractions</t>
+  </si>
+  <si>
+    <t>works well, but open question whether tagger will remove apostrophes as the beginning of clitics? (we currently rely on that for identificaiton)</t>
+  </si>
+  <si>
+    <t>Biber only allows for one or two intervening adverbs, we allow  for more</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1620,8 +1632,12 @@
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
@@ -1630,8 +1646,12 @@
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
@@ -1641,7 +1661,9 @@
         <v>54</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
@@ -1691,7 +1713,9 @@
         <v>59</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
@@ -1732,8 +1756,12 @@
       <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">

</xml_diff>

<commit_message>
Started second check on analyse_wh_word function, not done yet. Corrected some minor mistakes. One of the features seems so tricky to identify that we might have to drop it.
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA7FE5-6BF8-4615-84BB-5BEDDAAD9878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79064713-8F3E-4D20-896A-2EEFD2DCE17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="5500" windowWidth="11090" windowHeight="4300" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="200">
   <si>
     <t/>
   </si>
@@ -633,6 +633,18 @@
   </si>
   <si>
     <t>Biber only allows for one or two intervening adverbs, we allow  for more</t>
+  </si>
+  <si>
+    <t>appears to work well</t>
+  </si>
+  <si>
+    <t>serious problems here, catches unwanted stuff ("there's nothing good that can come from it", "I'm sure that's a …"), but also ignores some relevant examples without that ("I am glad you liked it")</t>
+  </si>
+  <si>
+    <t>Biber excludes contracted auxiliaries here. I don't see why and our code currently does not exclude them</t>
+  </si>
+  <si>
+    <t>I can't tell because the current taggeer will not tag the "that"s in my example sentences as WH…</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1200,8 +1212,12 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -1293,7 +1309,9 @@
         <v>21</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -1303,7 +1321,9 @@
         <v>22</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
@@ -1415,7 +1435,9 @@
       <c r="C34" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -1425,7 +1447,9 @@
         <v>34</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">

</xml_diff>

<commit_message>
Finished second check on analyse_wh_words function.
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79064713-8F3E-4D20-896A-2EEFD2DCE17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B85BBD-75BC-4DEC-BED7-BB732001FBC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="201">
   <si>
     <t/>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>I can't tell because the current taggeer will not tag the "that"s in my example sentences as WH…</t>
+  </si>
+  <si>
+    <t>works really well, some problems related to the tagger (catches "fuck that shit" because shit is tagged as a verb… ^^)</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,7 +1396,9 @@
         <v>29</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -1403,7 +1408,9 @@
         <v>30</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -1413,7 +1420,9 @@
         <v>31</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
@@ -1423,7 +1432,9 @@
         <v>32</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">

</xml_diff>

<commit_message>
Started second check on the analyse_verb function, added code for finding imperatives, still a lot to do!
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B85BBD-75BC-4DEC-BED7-BB732001FBC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A7BBF-3D5F-4EFC-B83A-6B580C2EC750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Tabelle2!$A$2:$B$81</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Tabelle2!$A$2:$B$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="209">
   <si>
     <t/>
   </si>
@@ -53,9 +53,6 @@
     <t xml:space="preserve"> verbs in past tense</t>
   </si>
   <si>
-    <t xml:space="preserve"> verbs in perfect aspect</t>
-  </si>
-  <si>
     <t xml:space="preserve"> verbs in present tense</t>
   </si>
   <si>
@@ -299,18 +296,12 @@
     <t>Recall</t>
   </si>
   <si>
-    <t>we intentionally only use the first of the two conditions that Biber proposes for finding past tense verbs</t>
-  </si>
-  <si>
     <t>we use the POS-tag,  Biber suggests a list of prepositions instead</t>
   </si>
   <si>
     <t>"vpast_001"</t>
   </si>
   <si>
-    <t>"vperfect_002"</t>
-  </si>
-  <si>
     <t>"vpresent_003"</t>
   </si>
   <si>
@@ -644,10 +635,43 @@
     <t>Biber excludes contracted auxiliaries here. I don't see why and our code currently does not exclude them</t>
   </si>
   <si>
-    <t>I can't tell because the current taggeer will not tag the "that"s in my example sentences as WH…</t>
-  </si>
-  <si>
     <t>works really well, some problems related to the tagger (catches "fuck that shit" because shit is tagged as a verb… ^^)</t>
+  </si>
+  <si>
+    <t>instead of Biber's conditions we use the tag that identifies past tense verbs</t>
+  </si>
+  <si>
+    <t>"vpresperfect_002a"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verbs in present perfect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verbs in past perfect</t>
+  </si>
+  <si>
+    <t>"vpastperfect_002b"</t>
+  </si>
+  <si>
+    <t>Biber only looks for perfect aspect, we draw a finer distinction between present and past perfect. If we want to we can easily combine them later</t>
+  </si>
+  <si>
+    <t>instead of Biber's condition we use the tag to identify infinitives, which likely also catches some wrong imperatives</t>
+  </si>
+  <si>
+    <t>I can't tell because the current tagger will not tag the "that"s in my example sentences as WH…</t>
+  </si>
+  <si>
+    <t>lots of wrong hits, but all appear to be tagger-related</t>
+  </si>
+  <si>
+    <t>catches what it should, which is not much</t>
+  </si>
+  <si>
+    <t>currently we are implementing this as Biber intended, but it would make sense to look for further instances of ing-forms</t>
+  </si>
+  <si>
+    <t>(not included in Biber)</t>
   </si>
 </sst>
 </file>
@@ -730,7 +754,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40D99BE-96FE-4629-88D4-1F8802B80194}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D81" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E40D99BE-96FE-4629-88D4-1F8802B80194}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D82" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CD1E9984-ECA3-410E-BA89-2B6D8BFFC517}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{D21A4EB7-50A6-4AF1-85B1-4F1BD5983C4D}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
@@ -1038,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1053,862 +1077,878 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>197</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>199</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>179</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>196</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>188</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>172</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="D22" s="1" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="1" t="s">
-        <v>184</v>
-      </c>
+      <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1" t="s">
-        <v>184</v>
-      </c>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D55" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D65" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1" t="s">
-        <v>173</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>0</v>
@@ -1918,66 +1958,76 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C80" s="1"/>
-      <c r="D80" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued check on analyze_verb function
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A7BBF-3D5F-4EFC-B83A-6B580C2EC750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF760AB-1C86-42E5-A312-F54299095792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="213">
   <si>
     <t/>
   </si>
@@ -672,6 +672,18 @@
   </si>
   <si>
     <t>(not included in Biber)</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>not good, catches unintended stuff like "with prices going up" or "or is the passage saying something quite different" - might need to drop this one</t>
+  </si>
+  <si>
+    <t>currently can't check this due to tagger problems (tags the VBNs we are looking for as VBD)</t>
+  </si>
+  <si>
+    <t>some tagger inaccuracy</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1137,9 @@
       <c r="B4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1135,8 +1149,12 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1411,8 +1429,12 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -1421,8 +1443,12 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -1431,8 +1457,12 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -1784,7 +1814,9 @@
         <v>57</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
@@ -1973,7 +2005,9 @@
       <c r="B77" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -1983,7 +2017,9 @@
       <c r="B78" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C78" s="1"/>
+      <c r="C78" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -1993,7 +2029,9 @@
       <c r="B79" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C79" s="1"/>
+      <c r="C79" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -2003,7 +2041,9 @@
       <c r="B80" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="1"/>
+      <c r="C80" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -2013,7 +2053,9 @@
       <c r="B81" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D81" s="1" t="s">
         <v>172</v>
       </c>
@@ -2025,7 +2067,9 @@
       <c r="B82" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C82" s="1"/>
+      <c r="C82" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="D82" s="1" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Continued work on analyse_verb, added some open questions we need to discuss
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF760AB-1C86-42E5-A312-F54299095792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAB37FF-4316-4005-8E6D-6D3E6539074F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="217">
   <si>
     <t/>
   </si>
@@ -620,9 +620,6 @@
     <t>so far we only use the full forms (ought, should, must), while Biber also includes the contractions</t>
   </si>
   <si>
-    <t>works well, but open question whether tagger will remove apostrophes as the beginning of clitics? (we currently rely on that for identificaiton)</t>
-  </si>
-  <si>
     <t>Biber only allows for one or two intervening adverbs, we allow  for more</t>
   </si>
   <si>
@@ -684,6 +681,21 @@
   </si>
   <si>
     <t>some tagger inaccuracy</t>
+  </si>
+  <si>
+    <t>Biber only looks for perfect aspect, we draw a finer distinction between present and past perfect. If we want to we can easily combine them later.</t>
+  </si>
+  <si>
+    <t>Biber also includes prepositions as items following BE, we currently don't allow that. Instead we also include nouns.</t>
+  </si>
+  <si>
+    <t>this appears to catch everything it attempts to catch, but we might think about also including adverbs to the list to also count "I am really interested" etc</t>
+  </si>
+  <si>
+    <t>works well (tagger will not remove apostrophes!!)</t>
+  </si>
+  <si>
+    <t>instead of using Biber's elaborate syntax, we simply look for apostrophes</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
@@ -1112,35 +1124,39 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1150,10 +1166,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1272,10 +1288,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1343,8 +1359,12 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -1369,7 +1389,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1381,7 +1401,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1402,10 +1422,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1416,10 +1436,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1430,10 +1450,10 @@
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1444,10 +1464,10 @@
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1458,10 +1478,10 @@
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1473,7 +1493,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1485,7 +1505,7 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1497,7 +1517,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1509,7 +1529,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1523,7 +1543,7 @@
         <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1535,7 +1555,7 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1825,9 +1845,11 @@
       <c r="B61" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="D61" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1870,7 +1892,7 @@
         <v>62</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>181</v>
@@ -1972,10 +1994,10 @@
         <v>71</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -2006,7 +2028,7 @@
         <v>72</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D77" s="1"/>
     </row>
@@ -2018,7 +2040,7 @@
         <v>73</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D78" s="1"/>
     </row>
@@ -2030,7 +2052,7 @@
         <v>74</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D79" s="1"/>
     </row>
@@ -2042,7 +2064,7 @@
         <v>75</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D80" s="1"/>
     </row>
@@ -2054,7 +2076,7 @@
         <v>76</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>172</v>
@@ -2068,7 +2090,7 @@
         <v>77</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
Re-structured Raffaela's template for test sentences
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860834F6-1104-4894-8FB8-FCA26A7E7BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D969062-AD04-47C1-BC39-59D4419F206E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="593" yWindow="945" windowWidth="11437" windowHeight="11445" activeTab="1" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
-    <sheet name="R's template" sheetId="1" r:id="rId2"/>
+    <sheet name="Overview_precision_recall" sheetId="2" r:id="rId1"/>
+    <sheet name="Test_sentences" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Tabelle2!$A$2:$B$82</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Overview_precision_recall!$A$2:$B$82</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="401">
   <si>
     <t/>
   </si>
@@ -697,21 +705,6 @@
   </si>
   <si>
     <t>token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre-thought sentence </t>
-  </si>
-  <si>
-    <t>PT_count</t>
-  </si>
-  <si>
-    <t>PoS</t>
-  </si>
-  <si>
-    <t>realistic data</t>
-  </si>
-  <si>
-    <t>RD_count</t>
   </si>
   <si>
     <t>adverb</t>
@@ -1227,12 +1220,63 @@
   <si>
     <t>?most powerful</t>
   </si>
+  <si>
+    <t xml:space="preserve">sentence </t>
+  </si>
+  <si>
+    <t>sentence_type</t>
+  </si>
+  <si>
+    <t>authentic</t>
+  </si>
+  <si>
+    <t>negana_068</t>
+  </si>
+  <si>
+    <t>negana_069</t>
+  </si>
+  <si>
+    <t>negana_070</t>
+  </si>
+  <si>
+    <t>negana_071</t>
+  </si>
+  <si>
+    <t>negana_072</t>
+  </si>
+  <si>
+    <t>negana_073</t>
+  </si>
+  <si>
+    <t>negana_074</t>
+  </si>
+  <si>
+    <t>negana_075</t>
+  </si>
+  <si>
+    <t>negana_076</t>
+  </si>
+  <si>
+    <t>made-up</t>
+  </si>
+  <si>
+    <t>count_expected</t>
+  </si>
+  <si>
+    <t>count_observed</t>
+  </si>
+  <si>
+    <t>POS_expected</t>
+  </si>
+  <si>
+    <t>POS_observed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,8 +1299,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1275,6 +1331,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1288,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1307,9 +1369,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1363,7 +1441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1661,35 +1739,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
@@ -1703,7 +1782,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>197</v>
       </c>
@@ -1717,7 +1796,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>200</v>
       </c>
@@ -1731,7 +1810,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
@@ -1745,7 +1824,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -1759,7 +1838,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -1773,7 +1852,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
@@ -1785,7 +1864,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -1797,7 +1876,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
@@ -1809,7 +1888,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>91</v>
       </c>
@@ -1821,7 +1900,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
@@ -1833,7 +1912,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -1843,7 +1922,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -1853,7 +1932,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>95</v>
       </c>
@@ -1867,7 +1946,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>96</v>
       </c>
@@ -1879,7 +1958,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>97</v>
       </c>
@@ -1893,7 +1972,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -1905,7 +1984,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>99</v>
       </c>
@@ -1915,7 +1994,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
@@ -1925,7 +2004,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>101</v>
       </c>
@@ -1939,7 +2018,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>102</v>
       </c>
@@ -1953,7 +2032,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>103</v>
       </c>
@@ -1965,7 +2044,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -1977,7 +2056,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>105</v>
       </c>
@@ -1987,7 +2066,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>106</v>
       </c>
@@ -2001,7 +2080,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>107</v>
       </c>
@@ -2015,7 +2094,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>108</v>
       </c>
@@ -2029,7 +2108,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>109</v>
       </c>
@@ -2043,7 +2122,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
@@ -2057,7 +2136,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
@@ -2069,7 +2148,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
@@ -2081,7 +2160,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>113</v>
       </c>
@@ -2093,7 +2172,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
@@ -2105,7 +2184,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>115</v>
       </c>
@@ -2119,7 +2198,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>116</v>
       </c>
@@ -2131,7 +2210,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2143,7 +2222,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>118</v>
       </c>
@@ -2155,7 +2234,7 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>119</v>
       </c>
@@ -2165,7 +2244,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>120</v>
       </c>
@@ -2175,7 +2254,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -2187,7 +2266,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>122</v>
       </c>
@@ -2199,7 +2278,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>123</v>
       </c>
@@ -2213,7 +2292,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -2225,7 +2304,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>125</v>
       </c>
@@ -2235,7 +2314,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>126</v>
       </c>
@@ -2245,7 +2324,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
@@ -2257,7 +2336,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>128</v>
       </c>
@@ -2271,7 +2350,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -2281,7 +2360,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>130</v>
       </c>
@@ -2293,7 +2372,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>131</v>
       </c>
@@ -2303,7 +2382,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>132</v>
       </c>
@@ -2315,7 +2394,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>133</v>
       </c>
@@ -2329,7 +2408,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>134</v>
       </c>
@@ -2343,7 +2422,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>135</v>
       </c>
@@ -2357,7 +2436,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>136</v>
       </c>
@@ -2369,7 +2448,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>137</v>
       </c>
@@ -2379,7 +2458,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>138</v>
       </c>
@@ -2389,7 +2468,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>139</v>
       </c>
@@ -2399,7 +2478,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>140</v>
       </c>
@@ -2411,7 +2490,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>141</v>
       </c>
@@ -2425,7 +2504,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>142</v>
       </c>
@@ -2435,7 +2514,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>143</v>
       </c>
@@ -2447,7 +2526,7 @@
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>144</v>
       </c>
@@ -2457,7 +2536,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>145</v>
       </c>
@@ -2471,7 +2550,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>146</v>
       </c>
@@ -2483,7 +2562,7 @@
       </c>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>147</v>
       </c>
@@ -2495,7 +2574,7 @@
       </c>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>148</v>
       </c>
@@ -2507,7 +2586,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -2519,7 +2598,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>150</v>
       </c>
@@ -2529,7 +2608,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>151</v>
       </c>
@@ -2539,7 +2618,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>152</v>
       </c>
@@ -2549,7 +2628,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>153</v>
       </c>
@@ -2559,7 +2638,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>154</v>
       </c>
@@ -2573,7 +2652,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>155</v>
       </c>
@@ -2583,7 +2662,7 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>156</v>
       </c>
@@ -2593,7 +2672,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
@@ -2605,7 +2684,7 @@
       </c>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>158</v>
       </c>
@@ -2617,7 +2696,7 @@
       </c>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>159</v>
       </c>
@@ -2629,7 +2708,7 @@
       </c>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>160</v>
       </c>
@@ -2641,7 +2720,7 @@
       </c>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>161</v>
       </c>
@@ -2655,7 +2734,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2680,1204 +2759,2348 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49EAFD2-A476-43DD-A56A-ECCAF12AB833}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="23.28515625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9" style="3"/>
-    <col min="7" max="7" width="20.85546875" style="3" customWidth="1"/>
-    <col min="8" max="9" width="9" style="3"/>
+    <col min="1" max="1" width="10.54296875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="14.54296875" style="3"/>
+    <col min="4" max="4" width="9.81640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" style="3" customWidth="1"/>
+    <col min="8" max="11" width="14.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" t="s">
+        <v>370</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B18" t="s">
+        <v>370</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" t="s">
+        <v>370</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B20" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B21" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" t="s">
+        <v>370</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B24" t="s">
+        <v>370</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" t="s">
+        <v>370</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B26" t="s">
+        <v>370</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B27" t="s">
+        <v>370</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" t="s">
+        <v>357</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B29" t="s">
+        <v>357</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" t="s">
+        <v>357</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B31" t="s">
+        <v>357</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B32" t="s">
+        <v>357</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B33" t="s">
+        <v>357</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B34" t="s">
+        <v>377</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B35" t="s">
+        <v>377</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B36" t="s">
+        <v>377</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B37" t="s">
+        <v>377</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B38" t="s">
+        <v>377</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" t="s">
+        <v>377</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B40" t="s">
+        <v>377</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B41" t="s">
+        <v>377</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B42" t="s">
+        <v>377</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B43" t="s">
+        <v>377</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B44" t="s">
+        <v>377</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B45" t="s">
+        <v>377</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B46" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" t="s">
+        <v>248</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" t="s">
+        <v>248</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" t="s">
+        <v>248</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" t="s">
+        <v>248</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" t="s">
+        <v>262</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B53" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" t="s">
+        <v>262</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" t="s">
+        <v>262</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" t="s">
+        <v>262</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B60" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E60" s="3">
+        <f>$G$26</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B61" t="s">
+        <v>262</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B96" t="s">
         <v>221</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C96" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B97" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B98" t="s">
+        <v>221</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B99" t="s">
+        <v>221</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D99" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B100" t="s">
+        <v>221</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B101" t="s">
+        <v>387</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B102" t="s">
+        <v>388</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B103" t="s">
+        <v>389</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B104" t="s">
+        <v>390</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B105" t="s">
+        <v>391</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B106" t="s">
+        <v>392</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B107" t="s">
+        <v>393</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E107" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G107" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H107" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B108" t="s">
+        <v>394</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D108" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H108" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B109" t="s">
+        <v>395</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="C3" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="G109" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H109" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" t="s">
-        <v>253</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B12" t="s">
-        <v>253</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B14" t="s">
-        <v>267</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15"/>
-      <c r="C15" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16"/>
-      <c r="C16" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17"/>
-      <c r="C17" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18"/>
-      <c r="C18" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="G18" s="3" t="str">
-        <f>$H$18</f>
-        <v>count = 0</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22"/>
-      <c r="C22" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-      <c r="C23" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-      <c r="C24" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27"/>
-      <c r="C27" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28"/>
-      <c r="C28" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29"/>
-      <c r="C29" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32"/>
-      <c r="C32" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33"/>
-      <c r="C33" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34"/>
-      <c r="C34" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37"/>
-      <c r="C37" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38"/>
-      <c r="C38" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42"/>
-      <c r="G42" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43"/>
-      <c r="G43" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46"/>
-      <c r="D46" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47"/>
-      <c r="D47" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-      <c r="D48" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B50" t="s">
-        <v>362</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51"/>
-      <c r="C51" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52"/>
-      <c r="C52" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B54" t="s">
-        <v>375</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55"/>
-      <c r="C55" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56"/>
-      <c r="C56" s="3" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57"/>
-      <c r="C57" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58"/>
-      <c r="C58" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59"/>
-      <c r="C59" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B60" t="s">
-        <v>382</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="3" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="3" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="3" t="s">
-        <v>388</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K138">
+    <sortCondition ref="A2:A138"/>
+    <sortCondition ref="B2:B138"/>
+    <sortCondition ref="C2:C138"/>
+    <sortCondition ref="D2:D138"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Continued check on the analyze_verb function
Proposed an alternative way of finding pro-verb do, awaits judgement
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D969062-AD04-47C1-BC39-59D4419F206E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF334EB-987E-48C2-804E-C41D8B48D569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="454">
   <si>
     <t/>
   </si>
@@ -1270,6 +1270,165 @@
   </si>
   <si>
     <t>POS_observed</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
+    <t>vsplitaux_063</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>We have ultimately baked quietly.</t>
+  </si>
+  <si>
+    <t>The boat was originally built to last a lifetime</t>
+  </si>
+  <si>
+    <t>The journal had really reported on this for weeks.</t>
+  </si>
+  <si>
+    <t>was</t>
+  </si>
+  <si>
+    <t>had</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>I had not broken from my struggles.</t>
+  </si>
+  <si>
+    <t>I've always wondered why they couldn't provide a list</t>
+  </si>
+  <si>
+    <t>VBP</t>
+  </si>
+  <si>
+    <t>I've never seen it</t>
+  </si>
+  <si>
+    <t>VBD</t>
+  </si>
+  <si>
+    <t>I am honestly completely totally cleaning my room.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 've</t>
+  </si>
+  <si>
+    <t>like Biber we here currently only look for one or two intervening adverbs (suggestions on how to improve this are welcome)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is imperative to not be afraid. </t>
+  </si>
+  <si>
+    <t>To openly scold him is foolish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would like for us to really connect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">He wants to not pee his pants. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I intend for me partens to really not shout. </t>
+  </si>
+  <si>
+    <t>vsplitinf_062</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>scold</t>
+  </si>
+  <si>
+    <t>connect</t>
+  </si>
+  <si>
+    <t>pee</t>
+  </si>
+  <si>
+    <t>shout</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What he needs is to really honestly talk to him. </t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>work well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whoever did this should come forward. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you have done so, continue with the next step. </t>
+  </si>
+  <si>
+    <t>And them my mum did so.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really did that. </t>
+  </si>
+  <si>
+    <t>pverbdo_012</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>He really does that.</t>
+  </si>
+  <si>
+    <t>does</t>
+  </si>
+  <si>
+    <t>Instead of Biber's broad criteria we are currently looking for very specific contexts</t>
+  </si>
+  <si>
+    <t>catches most cases I would say</t>
+  </si>
+  <si>
+    <t>VBN</t>
+  </si>
+  <si>
+    <t>VBZ</t>
+  </si>
+  <si>
+    <t>… and very good at what he does</t>
+  </si>
+  <si>
+    <t>I really wish I could do this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I do love ice cream. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">And then he really did surprise me. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The plant does not grow. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">But then I did finally recognise him. </t>
+  </si>
+  <si>
+    <t>for the emphatic do + verb we allow for more intervening adverbs than Biber does</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1385,6 +1544,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1740,8 +1902,8 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1929,8 +2091,12 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -2379,8 +2545,12 @@
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
@@ -2533,8 +2703,12 @@
       <c r="B64" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
@@ -2759,11 +2933,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49EAFD2-A476-43DD-A56A-ECCAF12AB833}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5091,12 +5265,708 @@
         <v>225</v>
       </c>
     </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0</v>
+      </c>
+      <c r="G110" s="3">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="F111" s="3">
+        <v>1</v>
+      </c>
+      <c r="G111" s="3">
+        <v>1</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="F112" s="3">
+        <v>1</v>
+      </c>
+      <c r="G112" s="3">
+        <v>1</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3">
+        <v>0</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F114" s="3">
+        <v>1</v>
+      </c>
+      <c r="G114" s="3">
+        <v>1</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="F115" s="3">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3">
+        <v>1</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="F116" s="3">
+        <v>1</v>
+      </c>
+      <c r="G116" s="3">
+        <v>1</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="F117" s="3">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F118" s="3">
+        <v>1</v>
+      </c>
+      <c r="G118" s="3">
+        <v>1</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="F119" s="3">
+        <v>1</v>
+      </c>
+      <c r="G119" s="3">
+        <v>1</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0</v>
+      </c>
+      <c r="G120" s="3">
+        <v>0</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="F121" s="3">
+        <v>0</v>
+      </c>
+      <c r="G121" s="3">
+        <v>0</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F122" s="3">
+        <v>1</v>
+      </c>
+      <c r="G122" s="3">
+        <v>1</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="F123" s="3">
+        <v>1</v>
+      </c>
+      <c r="G123" s="3">
+        <v>1</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F124" s="3">
+        <v>1</v>
+      </c>
+      <c r="G124" s="3">
+        <v>1</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F125" s="3">
+        <v>1</v>
+      </c>
+      <c r="G125" s="3">
+        <v>1</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F126" s="3">
+        <v>0</v>
+      </c>
+      <c r="G126" s="3">
+        <v>0</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F127" s="3">
+        <v>1</v>
+      </c>
+      <c r="G127" s="3">
+        <v>1</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="F128" s="3">
+        <v>1</v>
+      </c>
+      <c r="G128" s="3">
+        <v>1</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F129" s="3">
+        <v>1</v>
+      </c>
+      <c r="G129" s="3">
+        <v>1</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F130" s="3">
+        <v>1</v>
+      </c>
+      <c r="G130" s="3">
+        <v>1</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F131" s="3">
+        <v>2</v>
+      </c>
+      <c r="G131" s="3">
+        <v>2</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="F132" s="3">
+        <v>0</v>
+      </c>
+      <c r="G132" s="3">
+        <v>0</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="F133" s="3">
+        <v>1</v>
+      </c>
+      <c r="G133" s="3">
+        <v>1</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K138">
-    <sortCondition ref="A2:A138"/>
-    <sortCondition ref="B2:B138"/>
-    <sortCondition ref="C2:C138"/>
-    <sortCondition ref="D2:D138"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K137">
+    <sortCondition ref="A2:A137"/>
+    <sortCondition ref="B2:B137"/>
+    <sortCondition ref="C2:C137"/>
+    <sortCondition ref="D2:D137"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed check on analyze_verb function, yeah!!
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF334EB-987E-48C2-804E-C41D8B48D569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA35C3F-AB46-4D31-BEB9-CACAAC152A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{48FFCA11-554B-42A9-96F9-0993B079C157}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="500">
   <si>
     <t/>
   </si>
@@ -1429,6 +1429,144 @@
   </si>
   <si>
     <t>for the emphatic do + verb we allow for more intervening adverbs than Biber does</t>
+  </si>
+  <si>
+    <t>He wrote John would come and stay.</t>
+  </si>
+  <si>
+    <t>Anna has promised my present will arrive in time.</t>
+  </si>
+  <si>
+    <t>He claimed green shorts look good on him.</t>
+  </si>
+  <si>
+    <t>thatdel_060</t>
+  </si>
+  <si>
+    <t>believe</t>
+  </si>
+  <si>
+    <t>wrote</t>
+  </si>
+  <si>
+    <t>claimed</t>
+  </si>
+  <si>
+    <t>promised</t>
+  </si>
+  <si>
+    <t>I've heard some people say they weren't thrilled …</t>
+  </si>
+  <si>
+    <t>I swear she farted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 ??? </t>
+  </si>
+  <si>
+    <t>I think you could share some</t>
+  </si>
+  <si>
+    <t>We heard you were talking shit and…</t>
+  </si>
+  <si>
+    <t>They believe it's their *right* to procreate</t>
+  </si>
+  <si>
+    <t>heard</t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>for the third formulae given by Biber we currently don't allow for that additional intervening adjective, otherwise the same</t>
+  </si>
+  <si>
+    <t>works reasonably well</t>
+  </si>
+  <si>
+    <t>none so far</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I know what you want. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">He realised who was responsible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarah was indicating why she didn't want to leave. </t>
+  </si>
+  <si>
+    <t>Just imagine how aweful she was to him.</t>
+  </si>
+  <si>
+    <t>whclause_23</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>realised</t>
+  </si>
+  <si>
+    <t>imagine</t>
+  </si>
+  <si>
+    <t>indicating</t>
+  </si>
+  <si>
+    <t>You can't possibly know how a person feels about…</t>
+  </si>
+  <si>
+    <t>Until I see how this all plays out</t>
+  </si>
+  <si>
+    <t>I don't know why this is such a …</t>
+  </si>
+  <si>
+    <t>VBG</t>
+  </si>
+  <si>
+    <t>see</t>
+  </si>
+  <si>
+    <t>catches what it should, which is not everything there is</t>
+  </si>
+  <si>
+    <t>currently we only look for Biber's condition a (the one with the intervening adverbs)</t>
+  </si>
+  <si>
+    <t>passagentl_017</t>
+  </si>
+  <si>
+    <t>He has been revived, had been training</t>
+  </si>
+  <si>
+    <t>It was recorded shortly after the ..</t>
+  </si>
+  <si>
+    <t>if the father isn't named he's not on the hook…</t>
+  </si>
+  <si>
+    <t>Then the men were welcomed</t>
+  </si>
+  <si>
+    <t>VBd</t>
+  </si>
+  <si>
+    <t>been</t>
+  </si>
+  <si>
+    <t>were</t>
+  </si>
+  <si>
+    <t>passby_018</t>
+  </si>
+  <si>
+    <t>I was horribly terribly wounded by this hamster</t>
+  </si>
+  <si>
+    <t>You will be greeted by our delegates</t>
   </si>
 </sst>
 </file>
@@ -1901,9 +2039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6755F629-DA21-419F-A671-900231CF4234}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2157,8 +2295,12 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
@@ -2167,8 +2309,12 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -2229,8 +2375,12 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -2625,8 +2775,12 @@
       <c r="B57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
@@ -2635,8 +2789,12 @@
       <c r="B58" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
@@ -2645,8 +2803,12 @@
       <c r="B59" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
@@ -2681,8 +2843,12 @@
       <c r="B62" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
@@ -2933,11 +3099,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49EAFD2-A476-43DD-A56A-ECCAF12AB833}">
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5959,6 +6125,597 @@
       </c>
       <c r="I133" s="3" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="F134" s="3">
+        <v>1</v>
+      </c>
+      <c r="G134" s="3">
+        <v>1</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A135" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F135" s="3">
+        <v>1</v>
+      </c>
+      <c r="G135" s="3">
+        <v>1</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A136" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F136" s="3">
+        <v>1</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="F137" s="3">
+        <v>1</v>
+      </c>
+      <c r="G137" s="3">
+        <v>1</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A138" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F138" s="3">
+        <v>1</v>
+      </c>
+      <c r="G138" s="3">
+        <v>1</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A139" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="F139" s="3">
+        <v>1</v>
+      </c>
+      <c r="G139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A140" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F140" s="3">
+        <v>1</v>
+      </c>
+      <c r="G140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A141" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="F141" s="3">
+        <v>1</v>
+      </c>
+      <c r="G141" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A142" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="F142" s="3">
+        <v>1</v>
+      </c>
+      <c r="G142" s="3">
+        <v>1</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A143" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D143" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="F143" s="3">
+        <v>1</v>
+      </c>
+      <c r="G143" s="3">
+        <v>1</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A144" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="F144" s="3">
+        <v>1</v>
+      </c>
+      <c r="G144" s="3">
+        <v>1</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A145" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="F145" s="3">
+        <v>1</v>
+      </c>
+      <c r="G145" s="3">
+        <v>1</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A146" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="F146" s="3">
+        <v>1</v>
+      </c>
+      <c r="G146" s="3">
+        <v>1</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F147" s="3">
+        <v>1</v>
+      </c>
+      <c r="G147" s="3">
+        <v>1</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="F148" s="3">
+        <v>1</v>
+      </c>
+      <c r="G148" s="3">
+        <v>1</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="F149" s="3">
+        <v>1</v>
+      </c>
+      <c r="G149" s="3">
+        <v>1</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="F150" s="3">
+        <v>1</v>
+      </c>
+      <c r="G150" s="3">
+        <v>1</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D151" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="F151" s="3">
+        <v>1</v>
+      </c>
+      <c r="G151" s="3">
+        <v>1</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="F152" s="3">
+        <v>1</v>
+      </c>
+      <c r="G152" s="3">
+        <v>1</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="F153" s="3">
+        <v>1</v>
+      </c>
+      <c r="G153" s="3">
+        <v>1</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="F154" s="3">
+        <v>1</v>
+      </c>
+      <c r="G154" s="3">
+        <v>1</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on missing features
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A882262-05A5-42F5-A56B-6F8A738838D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A95053-F1E5-4169-A49F-BA24AEBBDA8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="1330" windowWidth="12630" windowHeight="8470" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="570" windowWidth="5900" windowHeight="9630" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Test_sentences" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0">Overview_precision_recall!$A$2:$B$82</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0">Overview_precision_recall!$A$2:$B$85</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="556">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1688,6 +1688,24 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>emoticons</t>
+  </si>
+  <si>
+    <t>"emoticons_207"</t>
+  </si>
+  <si>
+    <t>strategic lenghtening</t>
+  </si>
+  <si>
+    <t>"lengthening_206"</t>
+  </si>
+  <si>
+    <t>community-specific acronyms or lexical items</t>
+  </si>
+  <si>
+    <t>"reddit_vocab_216"</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1902,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D82" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D85" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -2192,18 +2210,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="A1:B82"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.81640625" customWidth="1"/>
     <col min="2" max="2" width="32.453125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -3155,34 +3173,30 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>210</v>
+        <v>553</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>552</v>
+      </c>
+      <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>212</v>
+        <v>551</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>550</v>
+      </c>
+      <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>209</v>
@@ -3191,10 +3205,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>209</v>
@@ -3203,52 +3217,84 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>448</v>
+        <v>214</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>452</v>
+        <v>215</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>218</v>
-      </c>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>449</v>
+        <v>216</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>453</v>
+        <v>217</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>451</v>
-      </c>
-      <c r="B81" t="s">
-        <v>454</v>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>450</v>
-      </c>
-      <c r="B82" t="s">
-        <v>455</v>
+      <c r="D81" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>209</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>451</v>
+      </c>
+      <c r="B83" t="s">
+        <v>454</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>450</v>
+      </c>
+      <c r="B84" t="s">
+        <v>455</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>555</v>
+      </c>
+      <c r="B85" t="s">
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -3264,14 +3310,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7223C10B-8642-4163-B1BD-0866630178C4}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
     <col min="2" max="2" width="20.453125" customWidth="1"/>
     <col min="3" max="3" width="7.36328125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
@@ -4770,15 +4816,15 @@
         <v>206</v>
       </c>
       <c r="H73" t="e">
-        <f t="shared" ref="H73:H83" si="6">D73/(D73+F73)</f>
+        <f t="shared" ref="H73:H82" si="6">D73/(D73+F73)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I73" t="e">
-        <f t="shared" ref="I73:I83" si="7">D73/(D73+G73)</f>
+        <f t="shared" ref="I73:I82" si="7">D73/(D73+G73)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J73" t="e">
-        <f t="shared" ref="J73:J83" si="8">2*((H73*I73)/(H73+I73))</f>
+        <f t="shared" ref="J73:J82" si="8">2*((H73*I73)/(H73+I73))</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started working on cleaning up the remaining comments on the functions and adding the missing features (e.g. progressives, average word length)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A95053-F1E5-4169-A49F-BA24AEBBDA8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE6725-C5B0-4C6C-98E5-CFB127A96DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="570" windowWidth="5900" windowHeight="9630" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Test_sentences" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0">Overview_precision_recall!$A$2:$B$85</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0">Overview_precision_recall!$A$2:$B$87</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="560">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1706,6 +1706,18 @@
   </si>
   <si>
     <t>"reddit_vocab_216"</t>
+  </si>
+  <si>
+    <t>verb phrases in the progressive aspect</t>
+  </si>
+  <si>
+    <t>"vprogressive_217"</t>
+  </si>
+  <si>
+    <t>emojis (counted separately from emoticons)</t>
+  </si>
+  <si>
+    <t>"emojis_218"</t>
   </si>
 </sst>
 </file>
@@ -1902,7 +1914,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D85" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Appendix_FeatureTags" displayName="Appendix_FeatureTags" ref="A2:D87" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -2210,11 +2222,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3296,6 +3308,28 @@
       <c r="B85" t="s">
         <v>554</v>
       </c>
+      <c r="C85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>557</v>
+      </c>
+      <c r="B86" t="s">
+        <v>556</v>
+      </c>
+      <c r="C86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>559</v>
+      </c>
+      <c r="B87" t="s">
+        <v>558</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3308,11 +3342,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7223C10B-8642-4163-B1BD-0866630178C4}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4850,10 +4884,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>210</v>
+        <v>553</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>211</v>
+        <v>552</v>
       </c>
       <c r="H75" t="e">
         <f t="shared" si="6"/>
@@ -4870,10 +4904,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>212</v>
+        <v>551</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>213</v>
+        <v>550</v>
       </c>
       <c r="H76" t="e">
         <f t="shared" si="6"/>
@@ -4890,10 +4924,10 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
@@ -4910,10 +4944,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>
@@ -4930,10 +4964,10 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>448</v>
+        <v>214</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>452</v>
+        <v>215</v>
       </c>
       <c r="H79" t="e">
         <f t="shared" si="6"/>
@@ -4950,10 +4984,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>449</v>
+        <v>216</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>453</v>
+        <v>217</v>
       </c>
       <c r="H80" t="e">
         <f t="shared" si="6"/>
@@ -4969,11 +5003,11 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>451</v>
-      </c>
-      <c r="B81" t="s">
-        <v>454</v>
+      <c r="A81" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="H81" t="e">
         <f t="shared" si="6"/>
@@ -4989,11 +5023,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>450</v>
-      </c>
-      <c r="B82" t="s">
-        <v>455</v>
+      <c r="A82" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="H82" t="e">
         <f t="shared" si="6"/>
@@ -5006,6 +5040,46 @@
       <c r="J82" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>451</v>
+      </c>
+      <c r="B83" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>450</v>
+      </c>
+      <c r="B84" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>555</v>
+      </c>
+      <c r="B85" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>557</v>
+      </c>
+      <c r="B86" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>559</v>
+      </c>
+      <c r="B87" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued cleaning comments on POS-functions
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE6725-C5B0-4C6C-98E5-CFB127A96DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C7A99-4C38-4891-B388-0E20325DDE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="561">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1718,6 +1718,9 @@
   </si>
   <si>
     <t>"emojis_218"</t>
+  </si>
+  <si>
+    <t>included within various POS-functions to make sure we catch all of them</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2229,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2900,7 +2903,9 @@
       <c r="B52" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>560</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Continued cleaning up PoS-functions
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C7A99-4C38-4891-B388-0E20325DDE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D289469-96A2-4FDE-97CF-231B20A7C1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="5950" windowWidth="17860" windowHeight="5150" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="561">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1381,9 +1381,6 @@
     <t>You will be greeted by our delegates</t>
   </si>
   <si>
-    <t>for "rather", "else", and "altogether" we only look for them as part of the conjunct list (not separately whether they are ininital position followed by a comma as Biber does)</t>
-  </si>
-  <si>
     <t>"comparatives_syn_212"</t>
   </si>
   <si>
@@ -1721,6 +1718,9 @@
   </si>
   <si>
     <t>included within various POS-functions to make sure we catch all of them</t>
+  </si>
+  <si>
+    <t>for "rather" we only look for sentence-initial cases followed by a comma (Biber also looks for sentence-initial cases of "rather" followed by everything other than adj/adv)</t>
   </si>
 </sst>
 </file>
@@ -2228,8 +2228,8 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2780,7 +2780,7 @@
         <v>127</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>128</v>
@@ -2794,7 +2794,7 @@
         <v>130</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>131</v>
@@ -2840,7 +2840,7 @@
         <v>140</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>447</v>
+        <v>560</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>141</v>
@@ -2904,7 +2904,7 @@
         <v>153</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>12</v>
@@ -3190,20 +3190,20 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>209</v>
@@ -3272,10 +3272,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>209</v>
@@ -3286,10 +3286,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B83" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>209</v>
@@ -3297,10 +3297,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B84" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>209</v>
@@ -3308,10 +3308,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B85" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C85" t="s">
         <v>209</v>
@@ -3319,10 +3319,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B86" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C86" t="s">
         <v>209</v>
@@ -3330,10 +3330,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B87" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -3373,19 +3373,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>543</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>544</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>545</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>546</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>3</v>
@@ -3394,7 +3394,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -3405,7 +3405,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D2">
         <v>75</v>
@@ -3440,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -4889,10 +4889,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H75" t="e">
         <f t="shared" si="6"/>
@@ -4909,10 +4909,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H76" t="e">
         <f t="shared" si="6"/>
@@ -5009,10 +5009,10 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H81" t="e">
         <f t="shared" si="6"/>
@@ -5029,10 +5029,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H82" t="e">
         <f t="shared" si="6"/>
@@ -5049,42 +5049,42 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B83" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B84" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B85" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B86" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B87" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -5145,10 +5145,10 @@
         <v>228</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -5252,7 +5252,7 @@
         <v>237</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5281,7 +5281,7 @@
         <v>237</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
@@ -5310,7 +5310,7 @@
         <v>237</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -5339,7 +5339,7 @@
         <v>232</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F8" s="12">
         <v>1</v>
@@ -5354,7 +5354,7 @@
         <v>234</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -5371,7 +5371,7 @@
         <v>232</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F9" s="12">
         <v>1</v>
@@ -5386,7 +5386,7 @@
         <v>234</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -5418,7 +5418,7 @@
         <v>234</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -5479,7 +5479,7 @@
         <v>234</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -5511,7 +5511,7 @@
         <v>234</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -5569,7 +5569,7 @@
         <v>234</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -5577,16 +5577,16 @@
         <v>229</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
@@ -5595,13 +5595,13 @@
         <v>0</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -5609,16 +5609,16 @@
         <v>229</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
@@ -5627,10 +5627,10 @@
         <v>0</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -5640,16 +5640,16 @@
         <v>229</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
@@ -5658,14 +5658,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -5673,16 +5673,16 @@
         <v>229</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
@@ -5691,10 +5691,10 @@
         <v>0</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J19" s="7"/>
     </row>
@@ -5703,16 +5703,16 @@
         <v>229</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>232</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -5721,10 +5721,10 @@
         <v>1</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -5732,16 +5732,16 @@
         <v>229</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
@@ -5750,10 +5750,10 @@
         <v>1</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -5761,7 +5761,7 @@
         <v>229</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>246</v>
@@ -5770,7 +5770,7 @@
         <v>232</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
@@ -5779,13 +5779,13 @@
         <v>1</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -5793,7 +5793,7 @@
         <v>229</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>246</v>
@@ -5802,7 +5802,7 @@
         <v>237</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
@@ -5811,10 +5811,10 @@
         <v>1</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -5822,7 +5822,7 @@
         <v>229</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>247</v>
@@ -5831,7 +5831,7 @@
         <v>232</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
@@ -5840,10 +5840,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -5851,7 +5851,7 @@
         <v>229</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>247</v>
@@ -5860,7 +5860,7 @@
         <v>237</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
@@ -5869,10 +5869,10 @@
         <v>1</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -5880,7 +5880,7 @@
         <v>229</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>248</v>
@@ -5889,7 +5889,7 @@
         <v>232</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F26" s="7">
         <v>1</v>
@@ -5898,10 +5898,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -5909,7 +5909,7 @@
         <v>229</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>248</v>
@@ -5918,7 +5918,7 @@
         <v>237</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>276</v>
@@ -5938,7 +5938,7 @@
         <v>229</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>249</v>
@@ -5947,7 +5947,7 @@
         <v>232</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
@@ -5956,10 +5956,10 @@
         <v>0</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -5967,7 +5967,7 @@
         <v>229</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>249</v>
@@ -5976,7 +5976,7 @@
         <v>237</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
@@ -5985,10 +5985,10 @@
         <v>1</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -6014,13 +6014,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>253</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -6046,7 +6046,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>253</v>
@@ -6075,7 +6075,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>257</v>
@@ -6104,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>257</v>
@@ -6133,7 +6133,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>276</v>
@@ -6162,7 +6162,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>276</v>
@@ -6173,16 +6173,16 @@
         <v>229</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>232</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
@@ -6191,13 +6191,13 @@
         <v>0</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -6205,16 +6205,16 @@
         <v>229</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
@@ -6223,13 +6223,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -6237,16 +6237,16 @@
         <v>229</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>232</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
@@ -6255,13 +6255,13 @@
         <v>1</v>
       </c>
       <c r="H38" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -6269,16 +6269,16 @@
         <v>229</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
@@ -6287,13 +6287,13 @@
         <v>1</v>
       </c>
       <c r="H39" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>535</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -6301,7 +6301,7 @@
         <v>229</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>262</v>
@@ -6310,7 +6310,7 @@
         <v>232</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
@@ -6319,10 +6319,10 @@
         <v>1</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -6330,7 +6330,7 @@
         <v>229</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>262</v>
@@ -6339,7 +6339,7 @@
         <v>237</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
@@ -6348,10 +6348,10 @@
         <v>1</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -6359,16 +6359,16 @@
         <v>229</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>232</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F42" s="3">
         <v>3</v>
@@ -6377,10 +6377,10 @@
         <v>3</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -6388,16 +6388,16 @@
         <v>229</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
@@ -6406,10 +6406,10 @@
         <v>1</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -6417,7 +6417,7 @@
         <v>229</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>263</v>
@@ -6426,7 +6426,7 @@
         <v>232</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F44" s="3">
         <v>2</v>
@@ -6435,13 +6435,13 @@
         <v>1</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I44" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
@@ -6449,7 +6449,7 @@
         <v>229</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>263</v>
@@ -6458,7 +6458,7 @@
         <v>237</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
@@ -6467,10 +6467,10 @@
         <v>1</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -6478,7 +6478,7 @@
         <v>229</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>264</v>
@@ -6487,7 +6487,7 @@
         <v>232</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
@@ -6496,10 +6496,10 @@
         <v>1</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
@@ -6507,7 +6507,7 @@
         <v>229</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>264</v>
@@ -6516,7 +6516,7 @@
         <v>237</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F47" s="3">
         <v>1</v>
@@ -6525,10 +6525,10 @@
         <v>1</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
@@ -6539,7 +6539,7 @@
         <v>266</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>232</v>
@@ -6568,13 +6568,13 @@
         <v>266</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>237</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F49" s="12">
         <v>1</v>
@@ -6586,7 +6586,7 @@
         <v>276</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
@@ -6615,7 +6615,7 @@
         <v>276</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
@@ -6644,7 +6644,7 @@
         <v>276</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
@@ -6661,7 +6661,7 @@
         <v>232</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F52" s="12">
         <v>1</v>
@@ -6673,7 +6673,7 @@
         <v>276</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
@@ -6702,7 +6702,7 @@
         <v>276</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
@@ -6889,7 +6889,7 @@
         <v>273</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>232</v>
@@ -6907,7 +6907,7 @@
         <v>276</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
@@ -7013,7 +7013,7 @@
         <v>232</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F64" s="3">
         <v>1</v>
@@ -7025,7 +7025,7 @@
         <v>276</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -7054,7 +7054,7 @@
         <v>276</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -7413,7 +7413,7 @@
         <v>301</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>232</v>
@@ -7442,7 +7442,7 @@
         <v>301</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>237</v>
@@ -7489,7 +7489,7 @@
         <v>276</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
@@ -7506,7 +7506,7 @@
         <v>237</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F81" s="12">
         <v>1</v>
@@ -7608,7 +7608,7 @@
         <v>276</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
@@ -7640,7 +7640,7 @@
         <v>276</v>
       </c>
       <c r="J85" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
@@ -7701,7 +7701,7 @@
         <v>276</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
@@ -7733,7 +7733,7 @@
         <v>276</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
@@ -7750,7 +7750,7 @@
         <v>237</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F89" s="12">
         <v>1</v>
@@ -7765,10 +7765,10 @@
         <v>276</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
@@ -7800,7 +7800,7 @@
         <v>276</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
@@ -7832,7 +7832,7 @@
         <v>276</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
@@ -8093,10 +8093,10 @@
         <v>276</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
@@ -8125,7 +8125,7 @@
         <v>276</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -8154,7 +8154,7 @@
         <v>276</v>
       </c>
       <c r="I102" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -8214,7 +8214,7 @@
         <v>276</v>
       </c>
       <c r="I104" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J104" s="7"/>
     </row>
@@ -8294,7 +8294,7 @@
         <v>232</v>
       </c>
       <c r="E107" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F107" s="12">
         <v>1</v>
@@ -9210,10 +9210,10 @@
         <v>1</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I138" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
@@ -9239,10 +9239,10 @@
         <v>1</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I139" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
@@ -9268,13 +9268,13 @@
         <v>0</v>
       </c>
       <c r="H140" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J140" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
@@ -9300,10 +9300,10 @@
         <v>1</v>
       </c>
       <c r="H141" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I141" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
@@ -9329,10 +9329,10 @@
         <v>2</v>
       </c>
       <c r="H142" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I142" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
@@ -9358,10 +9358,10 @@
         <v>1</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I143" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
@@ -9387,10 +9387,10 @@
         <v>1</v>
       </c>
       <c r="H144" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I144" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.35">
@@ -9416,10 +9416,10 @@
         <v>1</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I145" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.35">
@@ -9801,10 +9801,10 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B159" s="14" t="s">
         <v>486</v>
-      </c>
-      <c r="B159" s="14" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.35">
@@ -9822,7 +9822,7 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B161" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.35">
@@ -9840,7 +9840,7 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B163" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.35">
@@ -9858,7 +9858,7 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B165" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.35">
@@ -9876,7 +9876,7 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B167" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.35">
@@ -9912,7 +9912,7 @@
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B171" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.35">
@@ -9930,7 +9930,7 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B173" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First go at manual feature coding (with three features)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41244EE-131D-4B93-A1A6-9F1984390D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44CD973-77C9-4761-A8AF-2AF56D9AD02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="370" yWindow="4860" windowWidth="17860" windowHeight="5150" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="564">
   <si>
     <t>Feature_name</t>
   </si>
@@ -2236,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3358,9 +3358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7223C10B-8642-4163-B1BD-0866630178C4}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87:B87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3803,17 +3803,23 @@
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H20" t="e">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>99</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" t="e">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" t="e">
+        <v>1</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -4603,17 +4609,23 @@
       <c r="B60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H60" t="e">
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>95</v>
+      </c>
+      <c r="H60">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I60" t="e">
+        <v>1</v>
+      </c>
+      <c r="I60">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J60" t="e">
+        <v>1</v>
+      </c>
+      <c r="J60">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -4802,6 +4814,15 @@
       </c>
       <c r="B70" s="2" t="s">
         <v>195</v>
+      </c>
+      <c r="C70" t="s">
+        <v>542</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>100</v>
       </c>
       <c r="H70" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
First proper manual feature coding after bug fix (vpast_001)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44CD973-77C9-4761-A8AF-2AF56D9AD02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D0C762-867C-4174-BDA2-0BFD2624BEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="563">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1667,9 +1667,6 @@
   </si>
   <si>
     <t>HM</t>
-  </si>
-  <si>
-    <t>RT</t>
   </si>
   <si>
     <t>emoticons</t>
@@ -2287,7 +2284,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -2301,7 +2298,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -2521,7 +2518,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
@@ -2777,7 +2774,7 @@
         <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D41" s="2"/>
     </row>
@@ -2849,7 +2846,7 @@
         <v>136</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>137</v>
@@ -2913,7 +2910,7 @@
         <v>149</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>11</v>
@@ -3089,7 +3086,7 @@
         <v>184</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>11</v>
@@ -3191,7 +3188,7 @@
         <v>203</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>8</v>
@@ -3199,20 +3196,20 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -3317,32 +3314,32 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B85" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C85" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B86" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C86" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B87" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -3359,8 +3356,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3416,29 +3413,17 @@
       <c r="C2" t="s">
         <v>542</v>
       </c>
-      <c r="D2">
-        <v>75</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
+      <c r="H2" t="e">
         <f>D2/(D2+F2)</f>
-        <v>0.88235294117647056</v>
-      </c>
-      <c r="I2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I2" t="e">
         <f>D2/(D2+G2)</f>
-        <v>0.9375</v>
-      </c>
-      <c r="J2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J2" t="e">
         <f>2*((H2*I2)/(H2+I2))</f>
-        <v>0.90909090909090906</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -3448,32 +3433,17 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>543</v>
-      </c>
-      <c r="D3">
-        <v>60</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="e">
         <f>D3/(D3+F3)</f>
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="I3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" t="e">
         <f>D3/(D3+G3)</f>
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="J3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" t="e">
         <f>2*((H3*I3)/(H3+I3))</f>
-        <v>0.92307692307692313</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -3803,23 +3773,17 @@
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>99</v>
-      </c>
-      <c r="H20">
+      <c r="H20" t="e">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" t="e">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -4609,23 +4573,17 @@
       <c r="B60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D60">
-        <v>5</v>
-      </c>
-      <c r="E60">
-        <v>95</v>
-      </c>
-      <c r="H60">
+      <c r="H60" t="e">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I60">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I60" t="e">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J60">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J60" t="e">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -4815,15 +4773,6 @@
       <c r="B70" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C70" t="s">
-        <v>542</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>100</v>
-      </c>
       <c r="H70" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4919,10 +4868,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H75" t="e">
         <f t="shared" si="6"/>
@@ -4939,10 +4888,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H76" t="e">
         <f t="shared" si="6"/>
@@ -5095,26 +5044,26 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B85" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B86" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B87" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further manual coding: vpresperfect_0021, profirpers_006, prosecpers_007, link_202, exthere_020
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D0C762-867C-4174-BDA2-0BFD2624BEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63B8A74-8113-4D29-95E9-CF90E2133EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8750" yWindow="60" windowWidth="10320" windowHeight="9860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="563">
   <si>
     <t>Feature_name</t>
   </si>
@@ -3356,8 +3356,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3433,6 +3433,9 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C3" t="s">
+        <v>542</v>
+      </c>
       <c r="H3" t="e">
         <f>D3/(D3+F3)</f>
         <v>#DIV/0!</v>
@@ -3533,6 +3536,9 @@
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C8" t="s">
+        <v>542</v>
+      </c>
       <c r="H8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3553,6 +3559,9 @@
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C9" t="s">
+        <v>542</v>
+      </c>
       <c r="H9" t="e">
         <f t="shared" ref="H9:H72" si="3">D9/(D9+F9)</f>
         <v>#DIV/0!</v>
@@ -3813,6 +3822,9 @@
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="C22" t="s">
+        <v>542</v>
+      </c>
       <c r="H22" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4792,6 +4804,9 @@
       </c>
       <c r="B71" s="2" t="s">
         <v>197</v>
+      </c>
+      <c r="C71" t="s">
+        <v>542</v>
       </c>
       <c r="H71" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Further manual coding: proit_009 and prothirdper_008
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63B8A74-8113-4D29-95E9-CF90E2133EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B1D151-BA4D-4160-AE6A-996C089C36A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8750" yWindow="60" windowWidth="10320" windowHeight="9860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="563">
   <si>
     <t>Feature_name</t>
   </si>
@@ -3356,8 +3356,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3582,6 +3582,9 @@
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C10" t="s">
+        <v>542</v>
+      </c>
       <c r="H10" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3601,6 +3604,9 @@
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>542</v>
       </c>
       <c r="H11" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Further manual coding: question_208, exclamation_209, and hashtags_201 (but this feature will probably need to be deleted, not enough hits)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B1D151-BA4D-4160-AE6A-996C089C36A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C697E04-F138-4609-BAFF-67E8CE527F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8750" yWindow="60" windowWidth="10320" windowHeight="9860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="563">
   <si>
     <t>Feature_name</t>
   </si>
@@ -3357,7 +3357,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4791,6 +4791,9 @@
       <c r="B70" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="C70" t="s">
+        <v>542</v>
+      </c>
       <c r="H70" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4934,6 +4937,9 @@
       <c r="B77" s="2" t="s">
         <v>206</v>
       </c>
+      <c r="C77" t="s">
+        <v>542</v>
+      </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -4953,6 +4959,9 @@
       </c>
       <c r="B78" s="2" t="s">
         <v>208</v>
+      </c>
+      <c r="C78" t="s">
+        <v>542</v>
       </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Continued manual feature coding
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16407092-1612-44B5-B615-964F2C410167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC42F2-2E8D-4033-AFC0-9F865D051178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="569">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1731,9 +1731,6 @@
   </si>
   <si>
     <t>same. Progressive verb phrases should also be considered present tense verb phrases. Will/going to should not be counted as present tense verb phrases.</t>
-  </si>
-  <si>
-    <t>HM (might need re-doing)</t>
   </si>
   <si>
     <t>combined with amplifiers into one feature! [for the emphatic do + verb we allow for more intervening adverbs than Biber does]</t>
@@ -1757,6 +1754,9 @@
   </si>
   <si>
     <t xml:space="preserve"> amplifiers (+emphatics)</t>
+  </si>
+  <si>
+    <t>HM (needs re-doing, code aborted with Decoding-Error before sufficient hits found)</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2275,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2924,7 +2924,7 @@
         <v>144</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>11</v>
@@ -2938,13 +2938,13 @@
         <v>146</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -3401,8 +3401,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3723,7 +3723,7 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>541</v>
+        <v>568</v>
       </c>
       <c r="H14" t="e">
         <f t="shared" si="3"/>
@@ -3869,7 +3869,7 @@
         <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>564</v>
+        <v>541</v>
       </c>
       <c r="H21" t="e">
         <f t="shared" si="3"/>
@@ -4435,7 +4435,7 @@
         <v>143</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H49" t="e">
         <f t="shared" si="3"/>
@@ -4497,6 +4497,9 @@
       <c r="B52" s="2" t="s">
         <v>153</v>
       </c>
+      <c r="C52" t="s">
+        <v>541</v>
+      </c>
       <c r="H52" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4537,6 +4540,9 @@
       <c r="B54" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="C54" t="s">
+        <v>541</v>
+      </c>
       <c r="H54" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4557,6 +4563,9 @@
       <c r="B55" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="C55" t="s">
+        <v>541</v>
+      </c>
       <c r="H55" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4577,6 +4586,9 @@
       <c r="B56" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="C56" t="s">
+        <v>541</v>
+      </c>
       <c r="H56" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4597,6 +4609,9 @@
       <c r="B57" s="2" t="s">
         <v>165</v>
       </c>
+      <c r="C57" t="s">
+        <v>568</v>
+      </c>
       <c r="H57" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4618,7 +4633,7 @@
         <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="H58" t="e">
         <f t="shared" si="3"/>
@@ -4639,6 +4654,9 @@
       </c>
       <c r="B59" s="2" t="s">
         <v>169</v>
+      </c>
+      <c r="C59" t="s">
+        <v>541</v>
       </c>
       <c r="H59" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
features that need to be discussed before manual checking
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3761E3-9EAF-4699-87E9-49087927CEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A41A2B0-2C5D-4CB9-86E5-B5E708830FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="1610" windowWidth="10320" windowHeight="6940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="577">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1761,12 +1759,33 @@
   <si>
     <t>missing??</t>
   </si>
+  <si>
+    <t>RT (re-do once Axel is done wiht the new function)</t>
+  </si>
+  <si>
+    <t>things to discuss</t>
+  </si>
+  <si>
+    <t>good to go</t>
+  </si>
+  <si>
+    <t>"comparatives_ana_214"</t>
+  </si>
+  <si>
+    <t>"superlatives_ana_215"</t>
+  </si>
+  <si>
+    <t>good to go?</t>
+  </si>
+  <si>
+    <t>things to discuss (or have we discussed this one already?)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1798,6 +1817,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1841,7 +1874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1887,9 +1920,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1986,7 +2021,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2289,14 +2324,14 @@
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="32.46484375" customWidth="1"/>
+    <col min="3" max="3" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2327,7 +2362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2341,7 +2376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2355,7 +2390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2369,7 +2404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2383,7 +2418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2397,7 +2432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2409,7 +2444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2433,7 +2468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2445,7 +2480,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2457,7 +2492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2482,7 +2517,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2496,7 +2531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2508,7 +2543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -2522,7 +2557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2534,7 +2569,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2548,7 +2583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -2562,7 +2597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -2576,7 +2611,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2590,7 +2625,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -2602,7 +2637,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2614,7 +2649,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2628,7 +2663,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2642,7 +2677,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2656,7 +2691,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2670,7 +2705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2684,7 +2719,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2698,7 +2733,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2710,7 +2745,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2722,7 +2757,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -2734,7 +2769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -2746,7 +2781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2760,7 +2795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -2772,7 +2807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2784,7 +2819,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -2796,7 +2831,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -2806,7 +2841,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -2818,7 +2853,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2830,7 +2865,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -2844,7 +2879,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -2858,7 +2893,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -2870,7 +2905,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>131</v>
       </c>
@@ -2880,7 +2915,7 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
@@ -2890,7 +2925,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2904,7 +2939,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -2918,7 +2953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
@@ -2928,7 +2963,7 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -2942,7 +2977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="18" t="s">
         <v>145</v>
       </c>
@@ -2959,7 +2994,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -2973,7 +3008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -2987,7 +3022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
@@ -3001,7 +3036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3015,7 +3050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>158</v>
       </c>
@@ -3027,7 +3062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>160</v>
       </c>
@@ -3041,7 +3076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -3055,7 +3090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
@@ -3069,7 +3104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>166</v>
       </c>
@@ -3081,7 +3116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -3095,7 +3130,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -3109,7 +3144,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>176</v>
       </c>
@@ -3121,7 +3156,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3135,7 +3170,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>182</v>
       </c>
@@ -3149,7 +3184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>184</v>
       </c>
@@ -3161,7 +3196,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>186</v>
       </c>
@@ -3173,7 +3208,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3185,7 +3220,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3197,7 +3232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
@@ -3207,7 +3242,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>195</v>
       </c>
@@ -3217,7 +3252,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
@@ -3227,7 +3262,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3237,7 +3272,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>201</v>
       </c>
@@ -3251,7 +3286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>545</v>
       </c>
@@ -3261,7 +3296,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>543</v>
       </c>
@@ -3271,7 +3306,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3283,7 +3318,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3295,7 +3330,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3307,7 +3342,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>210</v>
       </c>
@@ -3319,7 +3354,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>441</v>
       </c>
@@ -3333,7 +3368,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>442</v>
       </c>
@@ -3347,7 +3382,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>444</v>
       </c>
@@ -3358,7 +3393,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>443</v>
       </c>
@@ -3369,7 +3404,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>547</v>
       </c>
@@ -3380,7 +3415,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>549</v>
       </c>
@@ -3391,7 +3426,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>551</v>
       </c>
@@ -3413,22 +3448,22 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.46484375" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3460,7 +3495,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3483,7 +3518,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3506,7 +3541,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3526,7 +3561,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3549,7 +3584,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3572,7 +3607,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -3580,7 +3615,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="H7" t="e">
         <f t="shared" si="0"/>
@@ -3595,7 +3630,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3618,7 +3653,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3641,7 +3676,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3664,7 +3699,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3687,13 +3722,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C12" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H12" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3707,7 +3745,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3730,7 +3768,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3753,13 +3791,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="C15" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H15" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3773,7 +3814,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -3796,13 +3837,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="C17" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H17" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3816,13 +3860,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="C18" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3836,13 +3883,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="C19" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H19" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3856,13 +3906,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="C20" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H20" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3876,7 +3929,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -3899,7 +3952,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -3922,7 +3975,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -3942,13 +3995,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="C24" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H24" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3962,13 +4018,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="C25" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H25" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3982,13 +4041,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="C26" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H26" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4002,13 +4064,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="C27" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H27" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4022,13 +4087,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="C28" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4042,13 +4110,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="C29" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H29" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4062,13 +4133,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="C30" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H30" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4082,13 +4156,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="C31" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H31" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4102,13 +4179,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="C32" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H32" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4122,13 +4202,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="C33" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4142,13 +4225,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="C34" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H34" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4162,13 +4248,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="C35" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H35" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4182,13 +4271,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="C36" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4202,14 +4294,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>568</v>
       </c>
       <c r="H37" t="e">
@@ -4225,13 +4317,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>113</v>
       </c>
+      <c r="C38" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H38" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4245,13 +4340,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="C39" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H39" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4265,13 +4363,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="C40" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H40" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4285,7 +4386,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -4308,7 +4409,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -4331,7 +4432,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -4354,13 +4455,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="C44" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H44" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4374,13 +4478,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="C45" s="20" t="s">
+        <v>571</v>
+      </c>
       <c r="H45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4394,13 +4501,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="C46" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H46" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4414,13 +4524,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="C47" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H47" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4434,13 +4547,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="C48" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H48" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4454,13 +4570,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>567</v>
       </c>
+      <c r="C49" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H49" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4474,13 +4593,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C50" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H50" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4494,13 +4616,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="C51" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H51" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4514,7 +4639,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>152</v>
       </c>
@@ -4537,13 +4662,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>156</v>
       </c>
+      <c r="C53" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H53" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4557,7 +4685,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>158</v>
       </c>
@@ -4580,7 +4708,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>160</v>
       </c>
@@ -4603,7 +4731,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
@@ -4626,7 +4754,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>164</v>
       </c>
@@ -4649,7 +4777,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>166</v>
       </c>
@@ -4672,7 +4800,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>168</v>
       </c>
@@ -4695,13 +4823,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="C60" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H60" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4715,13 +4846,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="C61" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H61" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4735,13 +4869,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>179</v>
       </c>
+      <c r="C62" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H62" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4755,13 +4892,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>183</v>
       </c>
+      <c r="C63" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H63" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4775,13 +4915,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="C64" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H64" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4795,13 +4938,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>187</v>
       </c>
+      <c r="C65" s="20" t="s">
+        <v>576</v>
+      </c>
       <c r="H65" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4815,13 +4961,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="C66" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H66" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4835,13 +4984,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="C67" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H67" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4855,7 +5007,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>193</v>
       </c>
@@ -4878,7 +5030,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>195</v>
       </c>
@@ -4901,13 +5053,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="C70" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H70" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4921,13 +5076,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="C71" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H71" t="e">
         <f t="shared" ref="H71:H80" si="6">D71/(D71+F71)</f>
         <v>#DIV/0!</v>
@@ -4941,13 +5099,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="C72" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H72" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -4961,13 +5122,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>545</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>544</v>
       </c>
+      <c r="C73" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H73" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -4981,13 +5145,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>543</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>542</v>
       </c>
+      <c r="C74" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H74" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5001,7 +5168,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>204</v>
       </c>
@@ -5024,7 +5191,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>206</v>
       </c>
@@ -5047,13 +5214,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="C77" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5067,13 +5237,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>211</v>
       </c>
+      <c r="C78" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5087,13 +5260,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>441</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>445</v>
       </c>
+      <c r="C79" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5107,13 +5283,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>442</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>446</v>
       </c>
+      <c r="C80" s="21" t="s">
+        <v>572</v>
+      </c>
       <c r="H80" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5127,48 +5306,64 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>444</v>
+        <v>573</v>
       </c>
       <c r="B81" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81" s="21" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>443</v>
+        <v>574</v>
       </c>
       <c r="B82" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82" s="21" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>547</v>
       </c>
       <c r="B83" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83" s="21" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>549</v>
       </c>
       <c r="B84" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84" s="21" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>551</v>
       </c>
       <c r="B85" t="s">
         <v>550</v>
       </c>
+      <c r="C85" s="22" t="s">
+        <v>575</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5181,22 +5376,22 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="3"/>
-    <col min="4" max="4" width="9.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="55.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.08984375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" style="3"/>
+    <col min="4" max="4" width="9.06640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="55.06640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.46484375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.9296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.06640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>214</v>
       </c>
@@ -5231,7 +5426,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>223</v>
       </c>
@@ -5260,7 +5455,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>223</v>
       </c>
@@ -5289,7 +5484,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>223</v>
       </c>
@@ -5318,7 +5513,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>223</v>
       </c>
@@ -5347,7 +5542,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>223</v>
       </c>
@@ -5376,7 +5571,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>223</v>
       </c>
@@ -5405,7 +5600,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>223</v>
       </c>
@@ -5437,7 +5632,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>223</v>
       </c>
@@ -5469,7 +5664,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>223</v>
       </c>
@@ -5501,7 +5696,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>223</v>
       </c>
@@ -5530,7 +5725,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>223</v>
       </c>
@@ -5562,7 +5757,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>223</v>
       </c>
@@ -5594,7 +5789,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>223</v>
       </c>
@@ -5623,7 +5818,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>223</v>
       </c>
@@ -5652,7 +5847,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>223</v>
       </c>
@@ -5684,7 +5879,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>223</v>
       </c>
@@ -5715,7 +5910,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>223</v>
       </c>
@@ -5748,7 +5943,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>223</v>
       </c>
@@ -5778,7 +5973,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>223</v>
       </c>
@@ -5807,7 +6002,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>223</v>
       </c>
@@ -5836,7 +6031,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>223</v>
       </c>
@@ -5868,7 +6063,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>223</v>
       </c>
@@ -5897,7 +6092,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>223</v>
       </c>
@@ -5926,7 +6121,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>223</v>
       </c>
@@ -5955,7 +6150,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>223</v>
       </c>
@@ -5984,7 +6179,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>223</v>
       </c>
@@ -6013,7 +6208,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>223</v>
       </c>
@@ -6042,7 +6237,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>223</v>
       </c>
@@ -6071,7 +6266,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>223</v>
       </c>
@@ -6103,7 +6298,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>223</v>
       </c>
@@ -6132,7 +6327,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>223</v>
       </c>
@@ -6161,7 +6356,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>223</v>
       </c>
@@ -6190,7 +6385,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>223</v>
       </c>
@@ -6219,7 +6414,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>223</v>
       </c>
@@ -6248,7 +6443,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>223</v>
       </c>
@@ -6280,7 +6475,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>223</v>
       </c>
@@ -6312,7 +6507,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>223</v>
       </c>
@@ -6344,7 +6539,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>223</v>
       </c>
@@ -6376,7 +6571,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>223</v>
       </c>
@@ -6405,7 +6600,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>223</v>
       </c>
@@ -6434,7 +6629,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>223</v>
       </c>
@@ -6463,7 +6658,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>223</v>
       </c>
@@ -6492,7 +6687,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>223</v>
       </c>
@@ -6524,7 +6719,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>223</v>
       </c>
@@ -6553,7 +6748,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>223</v>
       </c>
@@ -6582,7 +6777,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>223</v>
       </c>
@@ -6611,7 +6806,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>259</v>
       </c>
@@ -6640,7 +6835,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>259</v>
       </c>
@@ -6669,7 +6864,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>259</v>
       </c>
@@ -6698,7 +6893,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>259</v>
       </c>
@@ -6727,7 +6922,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>259</v>
       </c>
@@ -6756,7 +6951,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>259</v>
       </c>
@@ -6785,7 +6980,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>259</v>
       </c>
@@ -6814,7 +7009,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>259</v>
       </c>
@@ -6843,7 +7038,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>259</v>
       </c>
@@ -6872,7 +7067,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>259</v>
       </c>
@@ -6901,7 +7096,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>259</v>
       </c>
@@ -6930,7 +7125,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>259</v>
       </c>
@@ -6961,7 +7156,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>259</v>
       </c>
@@ -6992,7 +7187,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>259</v>
       </c>
@@ -7021,7 +7216,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>259</v>
       </c>
@@ -7050,7 +7245,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>259</v>
       </c>
@@ -7079,7 +7274,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>259</v>
       </c>
@@ -7108,7 +7303,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>259</v>
       </c>
@@ -7137,7 +7332,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>259</v>
       </c>
@@ -7166,7 +7361,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>259</v>
       </c>
@@ -7195,7 +7390,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>259</v>
       </c>
@@ -7224,7 +7419,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>259</v>
       </c>
@@ -7253,7 +7448,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>259</v>
       </c>
@@ -7282,7 +7477,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>259</v>
       </c>
@@ -7311,7 +7506,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>259</v>
       </c>
@@ -7340,7 +7535,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>259</v>
       </c>
@@ -7369,7 +7564,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>259</v>
       </c>
@@ -7398,7 +7593,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>259</v>
       </c>
@@ -7427,7 +7622,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>259</v>
       </c>
@@ -7456,7 +7651,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>259</v>
       </c>
@@ -7485,7 +7680,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>259</v>
       </c>
@@ -7514,7 +7709,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>259</v>
       </c>
@@ -7543,7 +7738,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>259</v>
       </c>
@@ -7572,7 +7767,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>259</v>
       </c>
@@ -7601,7 +7796,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>259</v>
       </c>
@@ -7630,7 +7825,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>259</v>
       </c>
@@ -7659,7 +7854,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>259</v>
       </c>
@@ -7691,7 +7886,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>259</v>
       </c>
@@ -7723,7 +7918,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>259</v>
       </c>
@@ -7752,7 +7947,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>259</v>
       </c>
@@ -7784,7 +7979,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>259</v>
       </c>
@@ -7816,7 +8011,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>259</v>
       </c>
@@ -7851,7 +8046,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>259</v>
       </c>
@@ -7883,7 +8078,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>259</v>
       </c>
@@ -7915,7 +8110,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>259</v>
       </c>
@@ -7944,7 +8139,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>259</v>
       </c>
@@ -7973,7 +8168,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>259</v>
       </c>
@@ -8002,7 +8197,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>259</v>
       </c>
@@ -8031,7 +8226,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>259</v>
       </c>
@@ -8060,7 +8255,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>259</v>
       </c>
@@ -8089,7 +8284,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>259</v>
       </c>
@@ -8118,7 +8313,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>259</v>
       </c>
@@ -8147,7 +8342,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>259</v>
       </c>
@@ -8179,7 +8374,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>259</v>
       </c>
@@ -8208,7 +8403,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>259</v>
       </c>
@@ -8237,7 +8432,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>259</v>
       </c>
@@ -8268,7 +8463,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>259</v>
       </c>
@@ -8298,7 +8493,7 @@
       </c>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>259</v>
       </c>
@@ -8329,7 +8524,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>259</v>
       </c>
@@ -8360,7 +8555,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>259</v>
       </c>
@@ -8391,7 +8586,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>259</v>
       </c>
@@ -8422,7 +8617,7 @@
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>259</v>
       </c>
@@ -8453,7 +8648,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>259</v>
       </c>
@@ -8484,7 +8679,7 @@
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>259</v>
       </c>
@@ -8513,7 +8708,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>259</v>
       </c>
@@ -8542,7 +8737,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>259</v>
       </c>
@@ -8571,7 +8766,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>353</v>
       </c>
@@ -8600,7 +8795,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>353</v>
       </c>
@@ -8629,7 +8824,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="3" t="s">
         <v>353</v>
       </c>
@@ -8658,7 +8853,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>353</v>
       </c>
@@ -8687,7 +8882,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>353</v>
       </c>
@@ -8716,7 +8911,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>353</v>
       </c>
@@ -8745,7 +8940,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>353</v>
       </c>
@@ -8774,7 +8969,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>353</v>
       </c>
@@ -8803,7 +8998,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>353</v>
       </c>
@@ -8832,7 +9027,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>353</v>
       </c>
@@ -8861,7 +9056,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>353</v>
       </c>
@@ -8890,7 +9085,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>353</v>
       </c>
@@ -8919,7 +9114,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>353</v>
       </c>
@@ -8948,7 +9143,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>353</v>
       </c>
@@ -8977,7 +9172,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>353</v>
       </c>
@@ -9006,7 +9201,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>353</v>
       </c>
@@ -9035,7 +9230,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>353</v>
       </c>
@@ -9064,7 +9259,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>353</v>
       </c>
@@ -9093,7 +9288,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>353</v>
       </c>
@@ -9122,7 +9317,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>353</v>
       </c>
@@ -9151,7 +9346,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>353</v>
       </c>
@@ -9180,7 +9375,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>353</v>
       </c>
@@ -9209,7 +9404,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>353</v>
       </c>
@@ -9238,7 +9433,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>353</v>
       </c>
@@ -9267,7 +9462,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>353</v>
       </c>
@@ -9296,7 +9491,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>353</v>
       </c>
@@ -9325,7 +9520,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>353</v>
       </c>
@@ -9357,7 +9552,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>353</v>
       </c>
@@ -9386,7 +9581,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>353</v>
       </c>
@@ -9415,7 +9610,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>353</v>
       </c>
@@ -9444,7 +9639,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>353</v>
       </c>
@@ -9473,7 +9668,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>353</v>
       </c>
@@ -9502,7 +9697,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>353</v>
       </c>
@@ -9531,7 +9726,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>353</v>
       </c>
@@ -9560,7 +9755,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>353</v>
       </c>
@@ -9589,7 +9784,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>353</v>
       </c>
@@ -9618,7 +9813,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>353</v>
       </c>
@@ -9647,7 +9842,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>353</v>
       </c>
@@ -9676,7 +9871,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>353</v>
       </c>
@@ -9705,7 +9900,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>353</v>
       </c>
@@ -9734,7 +9929,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>353</v>
       </c>
@@ -9763,7 +9958,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>353</v>
       </c>
@@ -9792,7 +9987,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156" s="3" t="s">
         <v>353</v>
       </c>
@@ -9821,7 +10016,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>353</v>
       </c>
@@ -9850,7 +10045,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>353</v>
       </c>
@@ -9879,7 +10074,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>479</v>
       </c>
@@ -9887,7 +10082,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160" s="7"/>
       <c r="B160" s="14"/>
       <c r="C160" s="7"/>
@@ -9900,12 +10095,12 @@
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B161" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -9918,12 +10113,12 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B163" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -9936,12 +10131,12 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B165" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -9954,12 +10149,12 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B167" s="3" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -9972,12 +10167,12 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B169" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -9990,12 +10185,12 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B171" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -10008,7 +10203,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B173" s="3" t="s">
         <v>486</v>
       </c>

</xml_diff>

<commit_message>
one last "good to go"
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A41A2B0-2C5D-4CB9-86E5-B5E708830FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA663F12-48A9-4316-83B9-DEB3159E9FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="577">
   <si>
     <t>Feature_name</t>
   </si>
@@ -3449,7 +3449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3547,6 +3547,9 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>572</v>
       </c>
       <c r="H4" t="e">
         <f t="shared" ref="H4:H8" si="0">D4/(D4+F4)</f>

</xml_diff>

<commit_message>
Updating features that are "good to go"
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA663F12-48A9-4316-83B9-DEB3159E9FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E2CAA4-165A-4390-B723-C8ED376892C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1778,7 +1778,7 @@
     <t>good to go?</t>
   </si>
   <si>
-    <t>things to discuss (or have we discussed this one already?)</t>
+    <t xml:space="preserve">good to go (check meeting 01.04.2022 after testing if necessary) </t>
   </si>
 </sst>
 </file>
@@ -3448,14 +3448,14 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.46484375" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
@@ -3732,8 +3732,8 @@
       <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>571</v>
+      <c r="C12" s="21" t="s">
+        <v>572</v>
       </c>
       <c r="H12" t="e">
         <f t="shared" si="3"/>
@@ -3916,8 +3916,8 @@
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>571</v>
+      <c r="C20" s="22" t="s">
+        <v>576</v>
       </c>
       <c r="H20" t="e">
         <f t="shared" si="3"/>
@@ -4005,8 +4005,8 @@
       <c r="B24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>571</v>
+      <c r="C24" s="22" t="s">
+        <v>576</v>
       </c>
       <c r="H24" t="e">
         <f t="shared" si="3"/>
@@ -4097,8 +4097,8 @@
       <c r="B28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>571</v>
+      <c r="C28" s="22" t="s">
+        <v>576</v>
       </c>
       <c r="H28" t="e">
         <f t="shared" si="3"/>
@@ -4120,8 +4120,8 @@
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>571</v>
+      <c r="C29" s="22" t="s">
+        <v>576</v>
       </c>
       <c r="H29" t="e">
         <f t="shared" si="3"/>
@@ -4143,8 +4143,8 @@
       <c r="B30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>571</v>
+      <c r="C30" s="22" t="s">
+        <v>576</v>
       </c>
       <c r="H30" t="e">
         <f t="shared" si="3"/>
@@ -4948,8 +4948,8 @@
       <c r="B65" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C65" s="20" t="s">
-        <v>576</v>
+      <c r="C65" s="21" t="s">
+        <v>572</v>
       </c>
       <c r="H65" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Continued manual feature coding - half of the features already done! :)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036A574F-B7B9-4F05-83CD-206C9F54B985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD13995B-1E63-40DC-AFDE-26EA13BB46A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3440,8 +3440,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4526,8 +4526,8 @@
       <c r="B47" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>570</v>
+      <c r="C47" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="H47" t="e">
         <f t="shared" si="3"/>
@@ -4595,8 +4595,8 @@
       <c r="B50" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>570</v>
+      <c r="C50" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="H50" t="e">
         <f t="shared" si="3"/>
@@ -4757,7 +4757,7 @@
         <v>165</v>
       </c>
       <c r="C57" t="s">
-        <v>566</v>
+        <v>539</v>
       </c>
       <c r="H57" t="e">
         <f t="shared" si="3"/>
@@ -4780,7 +4780,7 @@
         <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>566</v>
+        <v>539</v>
       </c>
       <c r="H58" t="e">
         <f t="shared" si="3"/>
@@ -4963,8 +4963,8 @@
       <c r="B66" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C66" s="21" t="s">
-        <v>570</v>
+      <c r="C66" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="H66" t="e">
         <f t="shared" si="3"/>
@@ -4986,8 +4986,8 @@
       <c r="B67" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C67" s="21" t="s">
-        <v>570</v>
+      <c r="C67" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="H67" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
good to go features (updated)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD13995B-1E63-40DC-AFDE-26EA13BB46A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96070FBB-F3B8-4CC1-B857-56DF382D752A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="576">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1759,9 +1757,6 @@
     <t>RT (re-do once Axel is done wiht the new function)</t>
   </si>
   <si>
-    <t>things to discuss</t>
-  </si>
-  <si>
     <t>good to go</t>
   </si>
   <si>
@@ -1771,10 +1766,16 @@
     <t>"superlatives_ana_215"</t>
   </si>
   <si>
-    <t>good to go?</t>
-  </si>
-  <si>
     <t xml:space="preserve">good to go (check meeting 01.04.2022 after testing if necessary) </t>
+  </si>
+  <si>
+    <t>Axel is checking the function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good to go (discard in the likely case it is very innacurate) </t>
+  </si>
+  <si>
+    <t>doesn't need manual checking</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1921,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2017,7 +2018,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2320,14 +2321,14 @@
       <selection pane="bottomLeft" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="32.46484375" customWidth="1"/>
+    <col min="3" max="3" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2386,7 +2387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
@@ -2499,7 +2500,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -2553,7 +2554,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2659,7 +2660,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2701,7 +2702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2715,7 +2716,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2815,7 +2816,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -2827,7 +2828,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -2837,7 +2838,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -2849,7 +2850,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2861,7 +2862,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -2875,7 +2876,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -2901,7 +2902,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>131</v>
       </c>
@@ -2911,7 +2912,7 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
@@ -2921,7 +2922,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
@@ -2959,7 +2960,7 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="18" t="s">
         <v>145</v>
       </c>
@@ -2990,7 +2991,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3046,7 +3047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>158</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>160</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -3086,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>166</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>176</v>
       </c>
@@ -3152,7 +3153,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>182</v>
       </c>
@@ -3180,7 +3181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>184</v>
       </c>
@@ -3192,7 +3193,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>186</v>
       </c>
@@ -3204,7 +3205,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3228,7 +3229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
@@ -3238,7 +3239,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>195</v>
       </c>
@@ -3248,7 +3249,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
@@ -3258,7 +3259,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3268,7 +3269,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>201</v>
       </c>
@@ -3282,7 +3283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>543</v>
       </c>
@@ -3292,7 +3293,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>541</v>
       </c>
@@ -3302,7 +3303,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3314,7 +3315,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3326,7 +3327,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3338,7 +3339,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>210</v>
       </c>
@@ -3350,7 +3351,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>439</v>
       </c>
@@ -3362,7 +3363,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>440</v>
       </c>
@@ -3374,7 +3375,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>442</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>441</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>545</v>
       </c>
@@ -3407,7 +3408,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>547</v>
       </c>
@@ -3418,7 +3419,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>549</v>
       </c>
@@ -3440,22 +3441,22 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3487,7 +3488,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3510,7 +3511,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3533,7 +3534,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H4" t="e">
         <f t="shared" ref="H4:H8" si="0">D4/(D4+F4)</f>
@@ -3556,7 +3557,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3579,7 +3580,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3602,14 +3603,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="21" t="s">
         <v>568</v>
       </c>
       <c r="H7" t="e">
@@ -3625,7 +3626,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3648,7 +3649,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3694,7 +3695,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H12" t="e">
         <f t="shared" si="3"/>
@@ -3740,7 +3741,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3763,7 +3764,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H15" t="e">
         <f t="shared" si="3"/>
@@ -3809,7 +3810,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H17" t="e">
         <f t="shared" si="3"/>
@@ -3855,7 +3856,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>55</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H18" t="e">
         <f t="shared" si="3"/>
@@ -3878,7 +3879,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>58</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H19" t="e">
         <f t="shared" si="3"/>
@@ -3901,7 +3902,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -3909,7 +3910,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H20" t="e">
         <f t="shared" si="3"/>
@@ -3924,7 +3925,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -3947,7 +3948,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -3970,13 +3971,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="C23" s="21" t="s">
+        <v>569</v>
+      </c>
       <c r="H23" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3990,7 +3994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -3998,7 +4002,7 @@
         <v>73</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H24" t="e">
         <f t="shared" si="3"/>
@@ -4013,7 +4017,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -4021,7 +4025,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H25" t="e">
         <f t="shared" si="3"/>
@@ -4036,7 +4040,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -4044,7 +4048,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H26" t="e">
         <f t="shared" si="3"/>
@@ -4059,7 +4063,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -4067,7 +4071,7 @@
         <v>84</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H27" t="e">
         <f t="shared" si="3"/>
@@ -4082,7 +4086,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -4090,7 +4094,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H28" t="e">
         <f t="shared" si="3"/>
@@ -4105,7 +4109,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -4113,7 +4117,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H29" t="e">
         <f t="shared" si="3"/>
@@ -4128,7 +4132,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -4136,7 +4140,7 @@
         <v>93</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H30" t="e">
         <f t="shared" si="3"/>
@@ -4151,14 +4155,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="21" t="s">
         <v>569</v>
       </c>
       <c r="H31" t="e">
@@ -4174,14 +4178,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="21" t="s">
         <v>569</v>
       </c>
       <c r="H32" t="e">
@@ -4197,7 +4201,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -4205,7 +4209,7 @@
         <v>101</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="H33" t="e">
         <f t="shared" si="3"/>
@@ -4220,7 +4224,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -4228,7 +4232,7 @@
         <v>103</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="H34" t="e">
         <f t="shared" si="3"/>
@@ -4243,7 +4247,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -4251,7 +4255,7 @@
         <v>105</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H35" t="e">
         <f t="shared" si="3"/>
@@ -4266,15 +4270,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>569</v>
+      <c r="C36" s="22" t="s">
+        <v>574</v>
       </c>
       <c r="H36" t="e">
         <f t="shared" si="3"/>
@@ -4289,7 +4293,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -4335,7 +4339,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -4358,7 +4362,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -4381,7 +4385,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -4404,7 +4408,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -4427,7 +4431,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -4450,7 +4454,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -4458,7 +4462,7 @@
         <v>129</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H44" t="e">
         <f t="shared" si="3"/>
@@ -4473,15 +4477,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="20" t="s">
-        <v>569</v>
+      <c r="C45" s="11" t="s">
+        <v>575</v>
       </c>
       <c r="H45" t="e">
         <f t="shared" si="3"/>
@@ -4496,7 +4500,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -4504,7 +4508,7 @@
         <v>136</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H46" t="e">
         <f t="shared" si="3"/>
@@ -4519,7 +4523,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -4542,7 +4546,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
@@ -4550,7 +4554,7 @@
         <v>142</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H48" t="e">
         <f t="shared" si="3"/>
@@ -4565,7 +4569,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
@@ -4573,7 +4577,7 @@
         <v>565</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H49" t="e">
         <f t="shared" si="3"/>
@@ -4588,7 +4592,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -4611,7 +4615,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>149</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>150</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H51" t="e">
         <f t="shared" si="3"/>
@@ -4634,7 +4638,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>152</v>
       </c>
@@ -4657,7 +4661,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
@@ -4680,7 +4684,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>158</v>
       </c>
@@ -4703,7 +4707,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>160</v>
       </c>
@@ -4726,7 +4730,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
@@ -4749,7 +4753,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>164</v>
       </c>
@@ -4772,7 +4776,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>166</v>
       </c>
@@ -4795,7 +4799,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>168</v>
       </c>
@@ -4818,7 +4822,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>172</v>
       </c>
@@ -4826,7 +4830,7 @@
         <v>173</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H60" t="e">
         <f t="shared" si="3"/>
@@ -4841,7 +4845,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>176</v>
       </c>
@@ -4849,7 +4853,7 @@
         <v>177</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H61" t="e">
         <f t="shared" si="3"/>
@@ -4864,7 +4868,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>178</v>
       </c>
@@ -4872,7 +4876,7 @@
         <v>179</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H62" t="e">
         <f t="shared" si="3"/>
@@ -4887,7 +4891,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>182</v>
       </c>
@@ -4895,7 +4899,7 @@
         <v>183</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H63" t="e">
         <f t="shared" si="3"/>
@@ -4910,7 +4914,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>184</v>
       </c>
@@ -4918,7 +4922,7 @@
         <v>185</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H64" t="e">
         <f t="shared" si="3"/>
@@ -4933,7 +4937,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
@@ -4941,7 +4945,7 @@
         <v>187</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H65" t="e">
         <f t="shared" si="3"/>
@@ -4956,7 +4960,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
@@ -5002,7 +5006,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>193</v>
       </c>
@@ -5025,7 +5029,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>195</v>
       </c>
@@ -5048,7 +5052,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>197</v>
       </c>
@@ -5071,7 +5075,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
@@ -5094,7 +5098,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>201</v>
       </c>
@@ -5117,7 +5121,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>543</v>
       </c>
@@ -5140,7 +5144,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>541</v>
       </c>
@@ -5163,7 +5167,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>204</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>206</v>
       </c>
@@ -5209,7 +5213,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>208</v>
       </c>
@@ -5217,7 +5221,7 @@
         <v>209</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
@@ -5232,7 +5236,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>210</v>
       </c>
@@ -5240,7 +5244,7 @@
         <v>211</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>
@@ -5255,7 +5259,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>439</v>
       </c>
@@ -5278,7 +5282,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>440</v>
       </c>
@@ -5286,7 +5290,7 @@
         <v>444</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H80" t="e">
         <f t="shared" si="6"/>
@@ -5301,9 +5305,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B81" t="s">
         <v>445</v>
@@ -5312,18 +5316,18 @@
         <v>539</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B82" t="s">
         <v>446</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>545</v>
       </c>
@@ -5331,10 +5335,10 @@
         <v>544</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>547</v>
       </c>
@@ -5342,18 +5346,18 @@
         <v>546</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>549</v>
       </c>
       <c r="B85" t="s">
         <v>548</v>
       </c>
-      <c r="C85" s="22" t="s">
-        <v>573</v>
+      <c r="C85" s="21" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -5371,22 +5375,22 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="3"/>
-    <col min="4" max="4" width="9.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="55.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.08984375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" style="3"/>
+    <col min="4" max="4" width="9.06640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="55.06640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.46484375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.9296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.06640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>221</v>
       </c>
@@ -5450,7 +5454,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>221</v>
       </c>
@@ -5479,7 +5483,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>221</v>
       </c>
@@ -5508,7 +5512,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>221</v>
       </c>
@@ -5537,7 +5541,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>221</v>
       </c>
@@ -5566,7 +5570,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -5595,7 +5599,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>221</v>
       </c>
@@ -5627,7 +5631,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>221</v>
       </c>
@@ -5659,7 +5663,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>221</v>
       </c>
@@ -5691,7 +5695,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>221</v>
       </c>
@@ -5720,7 +5724,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>221</v>
       </c>
@@ -5752,7 +5756,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>221</v>
       </c>
@@ -5784,7 +5788,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>221</v>
       </c>
@@ -5813,7 +5817,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>221</v>
       </c>
@@ -5842,7 +5846,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>221</v>
       </c>
@@ -5874,7 +5878,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>221</v>
       </c>
@@ -5905,7 +5909,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>221</v>
       </c>
@@ -5938,7 +5942,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>221</v>
       </c>
@@ -5968,7 +5972,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>221</v>
       </c>
@@ -5997,7 +6001,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>221</v>
       </c>
@@ -6026,7 +6030,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>221</v>
       </c>
@@ -6058,7 +6062,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>221</v>
       </c>
@@ -6087,7 +6091,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>221</v>
       </c>
@@ -6116,7 +6120,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>221</v>
       </c>
@@ -6145,7 +6149,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>221</v>
       </c>
@@ -6174,7 +6178,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>221</v>
       </c>
@@ -6203,7 +6207,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>221</v>
       </c>
@@ -6232,7 +6236,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>221</v>
       </c>
@@ -6261,7 +6265,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -6293,7 +6297,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -6322,7 +6326,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>221</v>
       </c>
@@ -6351,7 +6355,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>221</v>
       </c>
@@ -6380,7 +6384,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>221</v>
       </c>
@@ -6409,7 +6413,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>221</v>
       </c>
@@ -6438,7 +6442,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>221</v>
       </c>
@@ -6470,7 +6474,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>221</v>
       </c>
@@ -6502,7 +6506,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>221</v>
       </c>
@@ -6534,7 +6538,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>221</v>
       </c>
@@ -6566,7 +6570,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>221</v>
       </c>
@@ -6595,7 +6599,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>221</v>
       </c>
@@ -6624,7 +6628,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>221</v>
       </c>
@@ -6653,7 +6657,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>221</v>
       </c>
@@ -6682,7 +6686,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>221</v>
       </c>
@@ -6714,7 +6718,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>221</v>
       </c>
@@ -6743,7 +6747,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>221</v>
       </c>
@@ -6772,7 +6776,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>221</v>
       </c>
@@ -6801,7 +6805,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>257</v>
       </c>
@@ -6830,7 +6834,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>257</v>
       </c>
@@ -6859,7 +6863,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>257</v>
       </c>
@@ -6888,7 +6892,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>257</v>
       </c>
@@ -6917,7 +6921,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>257</v>
       </c>
@@ -6946,7 +6950,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>257</v>
       </c>
@@ -6975,7 +6979,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>257</v>
       </c>
@@ -7004,7 +7008,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>257</v>
       </c>
@@ -7033,7 +7037,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>257</v>
       </c>
@@ -7062,7 +7066,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>257</v>
       </c>
@@ -7091,7 +7095,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>257</v>
       </c>
@@ -7120,7 +7124,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>257</v>
       </c>
@@ -7151,7 +7155,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>257</v>
       </c>
@@ -7182,7 +7186,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>257</v>
       </c>
@@ -7211,7 +7215,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>257</v>
       </c>
@@ -7240,7 +7244,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>257</v>
       </c>
@@ -7269,7 +7273,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>257</v>
       </c>
@@ -7298,7 +7302,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>257</v>
       </c>
@@ -7327,7 +7331,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>257</v>
       </c>
@@ -7356,7 +7360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>257</v>
       </c>
@@ -7385,7 +7389,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>257</v>
       </c>
@@ -7414,7 +7418,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>257</v>
       </c>
@@ -7443,7 +7447,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>257</v>
       </c>
@@ -7472,7 +7476,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>257</v>
       </c>
@@ -7501,7 +7505,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
@@ -7530,7 +7534,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>257</v>
       </c>
@@ -7559,7 +7563,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>257</v>
       </c>
@@ -7588,7 +7592,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>257</v>
       </c>
@@ -7617,7 +7621,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>257</v>
       </c>
@@ -7646,7 +7650,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>257</v>
       </c>
@@ -7675,7 +7679,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>257</v>
       </c>
@@ -7704,7 +7708,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>257</v>
       </c>
@@ -7733,7 +7737,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>257</v>
       </c>
@@ -7762,7 +7766,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>257</v>
       </c>
@@ -7791,7 +7795,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>257</v>
       </c>
@@ -7820,7 +7824,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>257</v>
       </c>
@@ -7849,7 +7853,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>257</v>
       </c>
@@ -7881,7 +7885,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>257</v>
       </c>
@@ -7913,7 +7917,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -7942,7 +7946,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>257</v>
       </c>
@@ -7974,7 +7978,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>257</v>
       </c>
@@ -8006,7 +8010,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>257</v>
       </c>
@@ -8041,7 +8045,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>257</v>
       </c>
@@ -8073,7 +8077,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>257</v>
       </c>
@@ -8105,7 +8109,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>257</v>
       </c>
@@ -8134,7 +8138,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>257</v>
       </c>
@@ -8163,7 +8167,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>257</v>
       </c>
@@ -8192,7 +8196,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>257</v>
       </c>
@@ -8221,7 +8225,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>257</v>
       </c>
@@ -8250,7 +8254,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>257</v>
       </c>
@@ -8279,7 +8283,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>257</v>
       </c>
@@ -8308,7 +8312,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>257</v>
       </c>
@@ -8337,7 +8341,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>257</v>
       </c>
@@ -8369,7 +8373,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>257</v>
       </c>
@@ -8398,7 +8402,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>257</v>
       </c>
@@ -8427,7 +8431,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>257</v>
       </c>
@@ -8458,7 +8462,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>257</v>
       </c>
@@ -8488,7 +8492,7 @@
       </c>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>257</v>
       </c>
@@ -8519,7 +8523,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>257</v>
       </c>
@@ -8550,7 +8554,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>257</v>
       </c>
@@ -8581,7 +8585,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>257</v>
       </c>
@@ -8612,7 +8616,7 @@
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
@@ -8643,7 +8647,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>257</v>
       </c>
@@ -8674,7 +8678,7 @@
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>257</v>
       </c>
@@ -8703,7 +8707,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>257</v>
       </c>
@@ -8732,7 +8736,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>257</v>
       </c>
@@ -8761,7 +8765,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>351</v>
       </c>
@@ -8790,7 +8794,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>351</v>
       </c>
@@ -8819,7 +8823,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="3" t="s">
         <v>351</v>
       </c>
@@ -8848,7 +8852,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>351</v>
       </c>
@@ -8877,7 +8881,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>351</v>
       </c>
@@ -8906,7 +8910,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>351</v>
       </c>
@@ -8935,7 +8939,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>351</v>
       </c>
@@ -8964,7 +8968,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>351</v>
       </c>
@@ -8993,7 +8997,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>351</v>
       </c>
@@ -9022,7 +9026,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>351</v>
       </c>
@@ -9051,7 +9055,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>351</v>
       </c>
@@ -9080,7 +9084,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>351</v>
       </c>
@@ -9109,7 +9113,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>351</v>
       </c>
@@ -9138,7 +9142,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>351</v>
       </c>
@@ -9167,7 +9171,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>351</v>
       </c>
@@ -9196,7 +9200,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>351</v>
       </c>
@@ -9225,7 +9229,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>351</v>
       </c>
@@ -9254,7 +9258,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>351</v>
       </c>
@@ -9283,7 +9287,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>351</v>
       </c>
@@ -9312,7 +9316,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>351</v>
       </c>
@@ -9341,7 +9345,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>351</v>
       </c>
@@ -9370,7 +9374,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>351</v>
       </c>
@@ -9399,7 +9403,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>351</v>
       </c>
@@ -9428,7 +9432,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>351</v>
       </c>
@@ -9457,7 +9461,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>351</v>
       </c>
@@ -9486,7 +9490,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>351</v>
       </c>
@@ -9515,7 +9519,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>351</v>
       </c>
@@ -9547,7 +9551,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>351</v>
       </c>
@@ -9576,7 +9580,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>351</v>
       </c>
@@ -9605,7 +9609,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>351</v>
       </c>
@@ -9634,7 +9638,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>351</v>
       </c>
@@ -9663,7 +9667,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>351</v>
       </c>
@@ -9692,7 +9696,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>351</v>
       </c>
@@ -9721,7 +9725,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>351</v>
       </c>
@@ -9750,7 +9754,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>351</v>
       </c>
@@ -9779,7 +9783,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>351</v>
       </c>
@@ -9808,7 +9812,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>351</v>
       </c>
@@ -9837,7 +9841,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>351</v>
       </c>
@@ -9866,7 +9870,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>351</v>
       </c>
@@ -9895,7 +9899,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>351</v>
       </c>
@@ -9924,7 +9928,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>351</v>
       </c>
@@ -9953,7 +9957,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>351</v>
       </c>
@@ -9982,7 +9986,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156" s="3" t="s">
         <v>351</v>
       </c>
@@ -10011,7 +10015,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>351</v>
       </c>
@@ -10040,7 +10044,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>351</v>
       </c>
@@ -10069,7 +10073,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>477</v>
       </c>
@@ -10077,7 +10081,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160" s="7"/>
       <c r="B160" s="14"/>
       <c r="C160" s="7"/>
@@ -10090,12 +10094,12 @@
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B161" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -10108,12 +10112,12 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B163" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -10126,12 +10130,12 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B165" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -10144,12 +10148,12 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B167" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -10162,12 +10166,12 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B169" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -10180,12 +10184,12 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B171" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -10198,7 +10202,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B173" s="3" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
manual coding: overview table update
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26185C8-3C05-433E-AE52-3063DB088F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797B7106-5781-4B52-AEA2-82CC1273C739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8078" yWindow="6975" windowWidth="15391" windowHeight="9533" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16665" yWindow="1185" windowWidth="13350" windowHeight="12690" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="ExterneDaten_1" localSheetId="0">Overview_precision_recall!$A$2:$B$87</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="579">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1782,6 +1782,9 @@
   </si>
   <si>
     <t>RT (but have doubts)</t>
+  </si>
+  <si>
+    <t>not gonna manual code</t>
   </si>
 </sst>
 </file>
@@ -2327,14 +2330,14 @@
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.796875" customWidth="1"/>
-    <col min="2" max="2" width="32.46484375" customWidth="1"/>
-    <col min="3" max="3" width="23.265625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2546,7 +2549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2572,7 +2575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -2600,7 +2603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -2614,7 +2617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2628,7 +2631,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2680,7 +2683,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2708,7 +2711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2736,7 +2739,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2760,7 +2763,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -2784,7 +2787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -2810,7 +2813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2822,7 +2825,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -2834,7 +2837,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -2844,7 +2847,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -2856,7 +2859,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2868,7 +2871,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -2908,7 +2911,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>131</v>
       </c>
@@ -2918,7 +2921,7 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
@@ -2928,7 +2931,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
@@ -2966,7 +2969,7 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>145</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>158</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>160</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>166</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>176</v>
       </c>
@@ -3159,7 +3162,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>182</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>184</v>
       </c>
@@ -3199,7 +3202,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>186</v>
       </c>
@@ -3211,7 +3214,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3235,7 +3238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
@@ -3245,7 +3248,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>195</v>
       </c>
@@ -3255,7 +3258,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
@@ -3265,7 +3268,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3275,7 +3278,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>201</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>543</v>
       </c>
@@ -3299,7 +3302,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>541</v>
       </c>
@@ -3309,7 +3312,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3321,7 +3324,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3333,7 +3336,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3345,7 +3348,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>210</v>
       </c>
@@ -3357,7 +3360,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>439</v>
       </c>
@@ -3369,7 +3372,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>440</v>
       </c>
@@ -3381,7 +3384,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>442</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>441</v>
       </c>
@@ -3403,7 +3406,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>545</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>547</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>549</v>
       </c>
@@ -3447,22 +3450,22 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3586,7 +3589,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3609,7 +3612,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3724,7 +3727,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3770,7 +3773,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3793,7 +3796,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -3839,7 +3842,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -3954,7 +3957,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -4000,7 +4003,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -4092,7 +4095,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -4115,7 +4118,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -4184,7 +4187,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -4207,7 +4210,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -4230,7 +4233,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -4253,7 +4256,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -4276,7 +4279,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -4345,7 +4348,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -4368,7 +4371,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -4437,7 +4440,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -4460,7 +4463,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -4483,7 +4486,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
@@ -4506,7 +4509,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -4529,7 +4532,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -4552,7 +4555,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
@@ -4575,7 +4578,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
@@ -4598,7 +4601,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>149</v>
       </c>
@@ -4644,7 +4647,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>152</v>
       </c>
@@ -4667,7 +4670,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
@@ -4690,7 +4693,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>158</v>
       </c>
@@ -4713,7 +4716,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>160</v>
       </c>
@@ -4736,7 +4739,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>164</v>
       </c>
@@ -4782,7 +4785,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>166</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>168</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>172</v>
       </c>
@@ -4851,7 +4854,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>176</v>
       </c>
@@ -4874,7 +4877,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>178</v>
       </c>
@@ -4897,7 +4900,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>182</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>184</v>
       </c>
@@ -4943,7 +4946,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
@@ -4966,7 +4969,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
@@ -5012,7 +5015,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>193</v>
       </c>
@@ -5035,7 +5038,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>195</v>
       </c>
@@ -5058,7 +5061,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>197</v>
       </c>
@@ -5081,7 +5084,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>201</v>
       </c>
@@ -5127,7 +5130,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>543</v>
       </c>
@@ -5150,7 +5153,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>541</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>204</v>
       </c>
@@ -5196,7 +5199,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>206</v>
       </c>
@@ -5219,15 +5222,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C77" s="21" t="s">
-        <v>569</v>
+      <c r="C77" s="11" t="s">
+        <v>578</v>
       </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
@@ -5242,15 +5245,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C78" s="21" t="s">
-        <v>569</v>
+      <c r="C78" s="11" t="s">
+        <v>578</v>
       </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>
@@ -5265,7 +5268,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>439</v>
       </c>
@@ -5288,7 +5291,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>440</v>
       </c>
@@ -5311,7 +5314,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>570</v>
       </c>
@@ -5322,7 +5325,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>571</v>
       </c>
@@ -5333,7 +5336,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>545</v>
       </c>
@@ -5344,7 +5347,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>547</v>
       </c>
@@ -5355,7 +5358,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>549</v>
       </c>
@@ -5381,22 +5384,22 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" style="3"/>
-    <col min="4" max="4" width="9.06640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="55.06640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.46484375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.9296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.06640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="3"/>
+    <col min="4" max="4" width="9" style="4" customWidth="1"/>
+    <col min="5" max="5" width="55" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
@@ -5431,7 +5434,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>221</v>
       </c>
@@ -5460,7 +5463,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>221</v>
       </c>
@@ -5489,7 +5492,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>221</v>
       </c>
@@ -5518,7 +5521,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>221</v>
       </c>
@@ -5547,7 +5550,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>221</v>
       </c>
@@ -5576,7 +5579,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -5605,7 +5608,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>221</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>221</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>221</v>
       </c>
@@ -5701,7 +5704,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>221</v>
       </c>
@@ -5730,7 +5733,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>221</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>221</v>
       </c>
@@ -5794,7 +5797,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>221</v>
       </c>
@@ -5823,7 +5826,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>221</v>
       </c>
@@ -5852,7 +5855,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>221</v>
       </c>
@@ -5884,7 +5887,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>221</v>
       </c>
@@ -5915,7 +5918,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>221</v>
       </c>
@@ -5948,7 +5951,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>221</v>
       </c>
@@ -5978,7 +5981,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>221</v>
       </c>
@@ -6007,7 +6010,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>221</v>
       </c>
@@ -6036,7 +6039,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>221</v>
       </c>
@@ -6068,7 +6071,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>221</v>
       </c>
@@ -6097,7 +6100,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>221</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>221</v>
       </c>
@@ -6155,7 +6158,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>221</v>
       </c>
@@ -6184,7 +6187,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>221</v>
       </c>
@@ -6213,7 +6216,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>221</v>
       </c>
@@ -6242,7 +6245,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>221</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -6303,7 +6306,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -6332,7 +6335,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>221</v>
       </c>
@@ -6361,7 +6364,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>221</v>
       </c>
@@ -6390,7 +6393,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>221</v>
       </c>
@@ -6419,7 +6422,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>221</v>
       </c>
@@ -6448,7 +6451,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>221</v>
       </c>
@@ -6480,7 +6483,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>221</v>
       </c>
@@ -6512,7 +6515,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>221</v>
       </c>
@@ -6544,7 +6547,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>221</v>
       </c>
@@ -6576,7 +6579,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>221</v>
       </c>
@@ -6605,7 +6608,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>221</v>
       </c>
@@ -6634,7 +6637,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>221</v>
       </c>
@@ -6663,7 +6666,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>221</v>
       </c>
@@ -6692,7 +6695,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>221</v>
       </c>
@@ -6724,7 +6727,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>221</v>
       </c>
@@ -6753,7 +6756,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>221</v>
       </c>
@@ -6782,7 +6785,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>221</v>
       </c>
@@ -6811,7 +6814,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>257</v>
       </c>
@@ -6840,7 +6843,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>257</v>
       </c>
@@ -6869,7 +6872,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>257</v>
       </c>
@@ -6898,7 +6901,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>257</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>257</v>
       </c>
@@ -6956,7 +6959,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>257</v>
       </c>
@@ -6985,7 +6988,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>257</v>
       </c>
@@ -7014,7 +7017,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>257</v>
       </c>
@@ -7043,7 +7046,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>257</v>
       </c>
@@ -7072,7 +7075,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>257</v>
       </c>
@@ -7101,7 +7104,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>257</v>
       </c>
@@ -7130,7 +7133,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>257</v>
       </c>
@@ -7161,7 +7164,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>257</v>
       </c>
@@ -7192,7 +7195,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>257</v>
       </c>
@@ -7221,7 +7224,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>257</v>
       </c>
@@ -7250,7 +7253,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>257</v>
       </c>
@@ -7279,7 +7282,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>257</v>
       </c>
@@ -7308,7 +7311,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>257</v>
       </c>
@@ -7337,7 +7340,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>257</v>
       </c>
@@ -7366,7 +7369,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>257</v>
       </c>
@@ -7395,7 +7398,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>257</v>
       </c>
@@ -7424,7 +7427,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>257</v>
       </c>
@@ -7453,7 +7456,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>257</v>
       </c>
@@ -7482,7 +7485,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>257</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
@@ -7540,7 +7543,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>257</v>
       </c>
@@ -7569,7 +7572,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>257</v>
       </c>
@@ -7598,7 +7601,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>257</v>
       </c>
@@ -7627,7 +7630,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>257</v>
       </c>
@@ -7656,7 +7659,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>257</v>
       </c>
@@ -7685,7 +7688,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>257</v>
       </c>
@@ -7714,7 +7717,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>257</v>
       </c>
@@ -7743,7 +7746,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>257</v>
       </c>
@@ -7772,7 +7775,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>257</v>
       </c>
@@ -7801,7 +7804,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>257</v>
       </c>
@@ -7830,7 +7833,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>257</v>
       </c>
@@ -7859,7 +7862,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>257</v>
       </c>
@@ -7891,7 +7894,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>257</v>
       </c>
@@ -7923,7 +7926,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -7952,7 +7955,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>257</v>
       </c>
@@ -7984,7 +7987,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>257</v>
       </c>
@@ -8016,7 +8019,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>257</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>257</v>
       </c>
@@ -8083,7 +8086,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>257</v>
       </c>
@@ -8115,7 +8118,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>257</v>
       </c>
@@ -8144,7 +8147,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>257</v>
       </c>
@@ -8173,7 +8176,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>257</v>
       </c>
@@ -8202,7 +8205,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>257</v>
       </c>
@@ -8231,7 +8234,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>257</v>
       </c>
@@ -8260,7 +8263,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>257</v>
       </c>
@@ -8289,7 +8292,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>257</v>
       </c>
@@ -8318,7 +8321,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>257</v>
       </c>
@@ -8347,7 +8350,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>257</v>
       </c>
@@ -8379,7 +8382,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>257</v>
       </c>
@@ -8408,7 +8411,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>257</v>
       </c>
@@ -8437,7 +8440,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>257</v>
       </c>
@@ -8468,7 +8471,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>257</v>
       </c>
@@ -8498,7 +8501,7 @@
       </c>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>257</v>
       </c>
@@ -8529,7 +8532,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>257</v>
       </c>
@@ -8560,7 +8563,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>257</v>
       </c>
@@ -8591,7 +8594,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>257</v>
       </c>
@@ -8622,7 +8625,7 @@
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
@@ -8653,7 +8656,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>257</v>
       </c>
@@ -8684,7 +8687,7 @@
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>257</v>
       </c>
@@ -8713,7 +8716,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>257</v>
       </c>
@@ -8742,7 +8745,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>257</v>
       </c>
@@ -8771,7 +8774,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>351</v>
       </c>
@@ -8800,7 +8803,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>351</v>
       </c>
@@ -8829,7 +8832,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>351</v>
       </c>
@@ -8858,7 +8861,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>351</v>
       </c>
@@ -8887,7 +8890,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>351</v>
       </c>
@@ -8916,7 +8919,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>351</v>
       </c>
@@ -8945,7 +8948,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>351</v>
       </c>
@@ -8974,7 +8977,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>351</v>
       </c>
@@ -9003,7 +9006,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>351</v>
       </c>
@@ -9032,7 +9035,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>351</v>
       </c>
@@ -9061,7 +9064,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>351</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>351</v>
       </c>
@@ -9119,7 +9122,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>351</v>
       </c>
@@ -9148,7 +9151,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>351</v>
       </c>
@@ -9177,7 +9180,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>351</v>
       </c>
@@ -9206,7 +9209,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>351</v>
       </c>
@@ -9235,7 +9238,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>351</v>
       </c>
@@ -9264,7 +9267,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>351</v>
       </c>
@@ -9293,7 +9296,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>351</v>
       </c>
@@ -9322,7 +9325,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>351</v>
       </c>
@@ -9351,7 +9354,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>351</v>
       </c>
@@ -9380,7 +9383,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>351</v>
       </c>
@@ -9409,7 +9412,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>351</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>351</v>
       </c>
@@ -9467,7 +9470,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>351</v>
       </c>
@@ -9496,7 +9499,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>351</v>
       </c>
@@ -9525,7 +9528,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>351</v>
       </c>
@@ -9557,7 +9560,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>351</v>
       </c>
@@ -9586,7 +9589,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>351</v>
       </c>
@@ -9615,7 +9618,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>351</v>
       </c>
@@ -9644,7 +9647,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>351</v>
       </c>
@@ -9673,7 +9676,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>351</v>
       </c>
@@ -9702,7 +9705,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>351</v>
       </c>
@@ -9731,7 +9734,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>351</v>
       </c>
@@ -9760,7 +9763,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>351</v>
       </c>
@@ -9789,7 +9792,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>351</v>
       </c>
@@ -9818,7 +9821,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>351</v>
       </c>
@@ -9847,7 +9850,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>351</v>
       </c>
@@ -9876,7 +9879,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>351</v>
       </c>
@@ -9905,7 +9908,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>351</v>
       </c>
@@ -9934,7 +9937,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>351</v>
       </c>
@@ -9963,7 +9966,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>351</v>
       </c>
@@ -9992,7 +9995,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>351</v>
       </c>
@@ -10021,7 +10024,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>351</v>
       </c>
@@ -10050,7 +10053,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>351</v>
       </c>
@@ -10079,7 +10082,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>477</v>
       </c>
@@ -10087,7 +10090,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
       <c r="B160" s="14"/>
       <c r="C160" s="7"/>
@@ -10100,12 +10103,12 @@
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -10118,12 +10121,12 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B163" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -10136,12 +10139,12 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B165" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -10154,12 +10157,12 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -10172,12 +10175,12 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -10190,12 +10193,12 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -10208,7 +10211,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
manual coding: overview table update (forgot sth, ops)
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797B7106-5781-4B52-AEA2-82CC1273C739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F42FA8-04FD-408C-B3DA-7DB39F7706BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16665" yWindow="1185" windowWidth="13350" windowHeight="12690" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9615" yWindow="1350" windowWidth="13350" windowHeight="12690" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -1781,10 +1781,10 @@
     <t>RT (in the making, takes forever to find them)</t>
   </si>
   <si>
-    <t>RT (but have doubts)</t>
-  </si>
-  <si>
     <t>not gonna manual code</t>
+  </si>
+  <si>
+    <t>RT (in the making)</t>
   </si>
 </sst>
 </file>
@@ -3450,8 +3450,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,7 +3735,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H12" t="e">
         <f t="shared" si="3"/>
@@ -4632,7 +4632,7 @@
         <v>150</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H51" t="e">
         <f t="shared" si="3"/>
@@ -5230,7 +5230,7 @@
         <v>209</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H77" t="e">
         <f t="shared" si="6"/>
@@ -5253,7 +5253,7 @@
         <v>211</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H78" t="e">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
update table for manual feature coding
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B466AD19-44AA-45E2-BA84-3F05C4E412C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D8E06-0389-41B8-9B42-012C975F454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -1753,9 +1751,6 @@
     <t>missing??</t>
   </si>
   <si>
-    <t>RT (re-do once Axel is done wiht the new function)</t>
-  </si>
-  <si>
     <t>good to go</t>
   </si>
   <si>
@@ -1793,6 +1788,9 @@
   </si>
   <si>
     <t xml:space="preserve"> (discard in the likely case it is very innacurate) </t>
+  </si>
+  <si>
+    <t>(re-do once Axel is done wiht the new function)</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1936,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2035,7 +2033,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2338,14 +2336,14 @@
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="32.46484375" customWidth="1"/>
+    <col min="3" max="3" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,7 +2360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2376,7 +2374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2404,7 +2402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2418,7 +2416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2446,7 +2444,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2458,7 +2456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2470,7 +2468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2494,7 +2492,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2506,7 +2504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2545,7 +2543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2557,7 +2555,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -2571,7 +2569,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2583,7 +2581,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2597,7 +2595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -2625,7 +2623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2639,7 +2637,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -2651,7 +2649,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2663,7 +2661,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2677,7 +2675,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2705,7 +2703,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2719,7 +2717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2733,7 +2731,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2747,7 +2745,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2759,7 +2757,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -2783,7 +2781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -2795,7 +2793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2809,7 +2807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -2821,7 +2819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2833,7 +2831,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -2845,7 +2843,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -2855,7 +2853,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -2867,7 +2865,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2879,7 +2877,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -2893,7 +2891,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -2907,7 +2905,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -2919,7 +2917,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>131</v>
       </c>
@@ -2929,7 +2927,7 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
@@ -2939,7 +2937,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2953,7 +2951,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
@@ -2977,7 +2975,7 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -2991,7 +2989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="18" t="s">
         <v>145</v>
       </c>
@@ -3008,7 +3006,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
@@ -3050,7 +3048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3064,7 +3062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>158</v>
       </c>
@@ -3076,7 +3074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>160</v>
       </c>
@@ -3090,7 +3088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -3104,7 +3102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
@@ -3118,7 +3116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>166</v>
       </c>
@@ -3130,7 +3128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -3144,7 +3142,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -3158,7 +3156,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>176</v>
       </c>
@@ -3170,7 +3168,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3184,7 +3182,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>182</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>184</v>
       </c>
@@ -3210,7 +3208,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>186</v>
       </c>
@@ -3222,7 +3220,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3234,7 +3232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3246,7 +3244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
@@ -3256,7 +3254,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>195</v>
       </c>
@@ -3266,7 +3264,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
@@ -3276,7 +3274,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3286,7 +3284,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>201</v>
       </c>
@@ -3300,7 +3298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>543</v>
       </c>
@@ -3310,7 +3308,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>541</v>
       </c>
@@ -3320,7 +3318,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3332,7 +3330,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3344,7 +3342,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3356,7 +3354,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>210</v>
       </c>
@@ -3368,7 +3366,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>439</v>
       </c>
@@ -3380,7 +3378,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>440</v>
       </c>
@@ -3392,7 +3390,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>442</v>
       </c>
@@ -3403,7 +3401,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>441</v>
       </c>
@@ -3414,7 +3412,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>545</v>
       </c>
@@ -3425,7 +3423,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>547</v>
       </c>
@@ -3436,7 +3434,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>549</v>
       </c>
@@ -3458,22 +3456,22 @@
   <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="4" width="7.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.265625" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
+    <col min="3" max="4" width="7.265625" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3505,7 +3503,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3528,7 +3526,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3551,7 +3549,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3559,7 +3557,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D4" s="21"/>
       <c r="I4" t="e">
@@ -3575,7 +3573,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3598,7 +3596,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3621,15 +3619,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>567</v>
+      <c r="C7" s="20" t="s">
+        <v>580</v>
       </c>
       <c r="D7" s="21"/>
       <c r="I7" t="e">
@@ -3645,7 +3643,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3668,7 +3666,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3691,7 +3689,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3714,7 +3712,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3737,7 +3735,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -3745,7 +3743,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D12" s="21"/>
       <c r="I12" t="e">
@@ -3761,7 +3759,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3784,7 +3782,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3807,7 +3805,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -3831,7 +3829,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -3854,7 +3852,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -3878,7 +3876,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -3902,7 +3900,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -3910,7 +3908,7 @@
         <v>58</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D19" s="21"/>
       <c r="I19" t="e">
@@ -3926,7 +3924,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -3937,7 +3935,7 @@
         <v>539</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I20" t="e">
         <f t="shared" si="3"/>
@@ -3952,7 +3950,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -3975,7 +3973,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -3998,7 +3996,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -4022,7 +4020,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -4033,7 +4031,7 @@
         <v>539</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I24" t="e">
         <f t="shared" si="3"/>
@@ -4048,7 +4046,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -4056,7 +4054,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D25" s="21"/>
       <c r="I25" t="e">
@@ -4072,7 +4070,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -4096,7 +4094,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -4120,7 +4118,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -4128,10 +4126,10 @@
         <v>88</v>
       </c>
       <c r="C28" s="21" t="s">
+        <v>576</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>577</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>578</v>
       </c>
       <c r="I28" t="e">
         <f t="shared" si="3"/>
@@ -4146,7 +4144,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -4154,10 +4152,10 @@
         <v>90</v>
       </c>
       <c r="C29" s="21" t="s">
+        <v>576</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>577</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>578</v>
       </c>
       <c r="I29" t="e">
         <f t="shared" si="3"/>
@@ -4172,7 +4170,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -4180,10 +4178,10 @@
         <v>93</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I30" t="e">
         <f t="shared" si="3"/>
@@ -4198,7 +4196,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -4222,7 +4220,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -4246,7 +4244,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -4254,7 +4252,7 @@
         <v>101</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D33" s="20"/>
       <c r="I33" t="e">
@@ -4270,7 +4268,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -4278,7 +4276,7 @@
         <v>103</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D34" s="20"/>
       <c r="I34" t="e">
@@ -4294,7 +4292,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -4302,7 +4300,7 @@
         <v>105</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D35" s="21"/>
       <c r="I35" t="e">
@@ -4318,7 +4316,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -4329,7 +4327,7 @@
         <v>539</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I36" t="e">
         <f t="shared" si="3"/>
@@ -4344,7 +4342,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -4368,7 +4366,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -4392,7 +4390,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -4416,7 +4414,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -4440,7 +4438,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -4463,7 +4461,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -4486,7 +4484,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -4509,7 +4507,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -4517,7 +4515,7 @@
         <v>129</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D44" s="21"/>
       <c r="I44" t="e">
@@ -4533,7 +4531,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
@@ -4541,7 +4539,7 @@
         <v>134</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D45" s="11"/>
       <c r="I45" t="e">
@@ -4557,7 +4555,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -4581,7 +4579,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -4605,7 +4603,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
@@ -4629,7 +4627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
@@ -4637,7 +4635,7 @@
         <v>565</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D49" s="21"/>
       <c r="I49" t="e">
@@ -4653,7 +4651,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -4677,7 +4675,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>149</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>150</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D51" s="21"/>
       <c r="I51" t="e">
@@ -4701,7 +4699,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>152</v>
       </c>
@@ -4724,7 +4722,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
@@ -4748,7 +4746,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>158</v>
       </c>
@@ -4771,7 +4769,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>160</v>
       </c>
@@ -4794,7 +4792,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
@@ -4817,7 +4815,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>164</v>
       </c>
@@ -4840,7 +4838,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>166</v>
       </c>
@@ -4863,7 +4861,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>168</v>
       </c>
@@ -4886,7 +4884,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>172</v>
       </c>
@@ -4910,7 +4908,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>176</v>
       </c>
@@ -4934,7 +4932,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>178</v>
       </c>
@@ -4958,7 +4956,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>182</v>
       </c>
@@ -4982,7 +4980,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>184</v>
       </c>
@@ -5006,7 +5004,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
@@ -5030,7 +5028,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
@@ -5054,7 +5052,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
@@ -5078,7 +5076,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>193</v>
       </c>
@@ -5101,7 +5099,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>195</v>
       </c>
@@ -5124,7 +5122,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>197</v>
       </c>
@@ -5148,7 +5146,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
@@ -5172,7 +5170,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>201</v>
       </c>
@@ -5196,7 +5194,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>543</v>
       </c>
@@ -5220,7 +5218,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>541</v>
       </c>
@@ -5244,7 +5242,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>204</v>
       </c>
@@ -5267,7 +5265,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>206</v>
       </c>
@@ -5290,7 +5288,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>208</v>
       </c>
@@ -5298,7 +5296,7 @@
         <v>209</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D77" s="11"/>
       <c r="I77" t="e">
@@ -5314,7 +5312,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>210</v>
       </c>
@@ -5322,7 +5320,7 @@
         <v>211</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D78" s="11"/>
       <c r="I78" t="e">
@@ -5338,7 +5336,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>439</v>
       </c>
@@ -5362,7 +5360,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>440</v>
       </c>
@@ -5386,9 +5384,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B81" t="s">
         <v>445</v>
@@ -5398,9 +5396,9 @@
       </c>
       <c r="D81" s="11"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B82" t="s">
         <v>446</v>
@@ -5410,7 +5408,7 @@
       </c>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>545</v>
       </c>
@@ -5418,11 +5416,11 @@
         <v>544</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D83" s="21"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>547</v>
       </c>
@@ -5434,7 +5432,7 @@
       </c>
       <c r="D84" s="11"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>549</v>
       </c>
@@ -5442,7 +5440,7 @@
         <v>548</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D85" s="21"/>
     </row>
@@ -5461,22 +5459,22 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="3"/>
+    <col min="1" max="1" width="9.73046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.53125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" style="3"/>
     <col min="4" max="4" width="9" style="4" customWidth="1"/>
     <col min="5" max="5" width="55" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.46484375" style="3" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
     <col min="8" max="8" width="8" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
@@ -5511,7 +5509,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>221</v>
       </c>
@@ -5540,7 +5538,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>221</v>
       </c>
@@ -5569,7 +5567,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>221</v>
       </c>
@@ -5598,7 +5596,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>221</v>
       </c>
@@ -5627,7 +5625,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>221</v>
       </c>
@@ -5656,7 +5654,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -5685,7 +5683,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>221</v>
       </c>
@@ -5717,7 +5715,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>221</v>
       </c>
@@ -5749,7 +5747,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>221</v>
       </c>
@@ -5781,7 +5779,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>221</v>
       </c>
@@ -5810,7 +5808,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>221</v>
       </c>
@@ -5842,7 +5840,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>221</v>
       </c>
@@ -5874,7 +5872,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>221</v>
       </c>
@@ -5903,7 +5901,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>221</v>
       </c>
@@ -5932,7 +5930,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>221</v>
       </c>
@@ -5964,7 +5962,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>221</v>
       </c>
@@ -5995,7 +5993,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>221</v>
       </c>
@@ -6028,7 +6026,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>221</v>
       </c>
@@ -6058,7 +6056,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>221</v>
       </c>
@@ -6087,7 +6085,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>221</v>
       </c>
@@ -6116,7 +6114,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>221</v>
       </c>
@@ -6148,7 +6146,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>221</v>
       </c>
@@ -6177,7 +6175,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>221</v>
       </c>
@@ -6206,7 +6204,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>221</v>
       </c>
@@ -6235,7 +6233,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>221</v>
       </c>
@@ -6264,7 +6262,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>221</v>
       </c>
@@ -6293,7 +6291,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>221</v>
       </c>
@@ -6322,7 +6320,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>221</v>
       </c>
@@ -6351,7 +6349,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -6383,7 +6381,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -6412,7 +6410,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>221</v>
       </c>
@@ -6441,7 +6439,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>221</v>
       </c>
@@ -6470,7 +6468,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>221</v>
       </c>
@@ -6499,7 +6497,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>221</v>
       </c>
@@ -6528,7 +6526,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>221</v>
       </c>
@@ -6560,7 +6558,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>221</v>
       </c>
@@ -6592,7 +6590,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>221</v>
       </c>
@@ -6624,7 +6622,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>221</v>
       </c>
@@ -6656,7 +6654,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>221</v>
       </c>
@@ -6685,7 +6683,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>221</v>
       </c>
@@ -6714,7 +6712,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>221</v>
       </c>
@@ -6743,7 +6741,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>221</v>
       </c>
@@ -6772,7 +6770,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>221</v>
       </c>
@@ -6804,7 +6802,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>221</v>
       </c>
@@ -6833,7 +6831,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>221</v>
       </c>
@@ -6862,7 +6860,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>221</v>
       </c>
@@ -6891,7 +6889,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>257</v>
       </c>
@@ -6920,7 +6918,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>257</v>
       </c>
@@ -6949,7 +6947,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>257</v>
       </c>
@@ -6978,7 +6976,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>257</v>
       </c>
@@ -7007,7 +7005,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>257</v>
       </c>
@@ -7036,7 +7034,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>257</v>
       </c>
@@ -7065,7 +7063,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>257</v>
       </c>
@@ -7094,7 +7092,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>257</v>
       </c>
@@ -7123,7 +7121,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>257</v>
       </c>
@@ -7152,7 +7150,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>257</v>
       </c>
@@ -7181,7 +7179,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>257</v>
       </c>
@@ -7210,7 +7208,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>257</v>
       </c>
@@ -7241,7 +7239,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>257</v>
       </c>
@@ -7272,7 +7270,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>257</v>
       </c>
@@ -7301,7 +7299,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>257</v>
       </c>
@@ -7330,7 +7328,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>257</v>
       </c>
@@ -7359,7 +7357,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>257</v>
       </c>
@@ -7388,7 +7386,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>257</v>
       </c>
@@ -7417,7 +7415,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>257</v>
       </c>
@@ -7446,7 +7444,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>257</v>
       </c>
@@ -7475,7 +7473,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>257</v>
       </c>
@@ -7504,7 +7502,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>257</v>
       </c>
@@ -7533,7 +7531,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>257</v>
       </c>
@@ -7562,7 +7560,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>257</v>
       </c>
@@ -7591,7 +7589,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
@@ -7620,7 +7618,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>257</v>
       </c>
@@ -7649,7 +7647,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>257</v>
       </c>
@@ -7678,7 +7676,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>257</v>
       </c>
@@ -7707,7 +7705,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>257</v>
       </c>
@@ -7736,7 +7734,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>257</v>
       </c>
@@ -7765,7 +7763,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>257</v>
       </c>
@@ -7794,7 +7792,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>257</v>
       </c>
@@ -7823,7 +7821,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>257</v>
       </c>
@@ -7852,7 +7850,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>257</v>
       </c>
@@ -7881,7 +7879,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>257</v>
       </c>
@@ -7910,7 +7908,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>257</v>
       </c>
@@ -7939,7 +7937,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>257</v>
       </c>
@@ -7971,7 +7969,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>257</v>
       </c>
@@ -8003,7 +8001,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -8032,7 +8030,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>257</v>
       </c>
@@ -8064,7 +8062,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>257</v>
       </c>
@@ -8096,7 +8094,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>257</v>
       </c>
@@ -8131,7 +8129,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>257</v>
       </c>
@@ -8163,7 +8161,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>257</v>
       </c>
@@ -8195,7 +8193,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>257</v>
       </c>
@@ -8224,7 +8222,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>257</v>
       </c>
@@ -8253,7 +8251,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>257</v>
       </c>
@@ -8282,7 +8280,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>257</v>
       </c>
@@ -8311,7 +8309,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>257</v>
       </c>
@@ -8340,7 +8338,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>257</v>
       </c>
@@ -8369,7 +8367,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>257</v>
       </c>
@@ -8398,7 +8396,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>257</v>
       </c>
@@ -8427,7 +8425,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>257</v>
       </c>
@@ -8459,7 +8457,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>257</v>
       </c>
@@ -8488,7 +8486,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>257</v>
       </c>
@@ -8517,7 +8515,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>257</v>
       </c>
@@ -8548,7 +8546,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>257</v>
       </c>
@@ -8578,7 +8576,7 @@
       </c>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>257</v>
       </c>
@@ -8609,7 +8607,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>257</v>
       </c>
@@ -8640,7 +8638,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>257</v>
       </c>
@@ -8671,7 +8669,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>257</v>
       </c>
@@ -8702,7 +8700,7 @@
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
@@ -8733,7 +8731,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>257</v>
       </c>
@@ -8764,7 +8762,7 @@
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>257</v>
       </c>
@@ -8793,7 +8791,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>257</v>
       </c>
@@ -8822,7 +8820,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>257</v>
       </c>
@@ -8851,7 +8849,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>351</v>
       </c>
@@ -8880,7 +8878,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>351</v>
       </c>
@@ -8909,7 +8907,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="3" t="s">
         <v>351</v>
       </c>
@@ -8938,7 +8936,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>351</v>
       </c>
@@ -8967,7 +8965,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>351</v>
       </c>
@@ -8996,7 +8994,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>351</v>
       </c>
@@ -9025,7 +9023,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>351</v>
       </c>
@@ -9054,7 +9052,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>351</v>
       </c>
@@ -9083,7 +9081,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>351</v>
       </c>
@@ -9112,7 +9110,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>351</v>
       </c>
@@ -9141,7 +9139,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>351</v>
       </c>
@@ -9170,7 +9168,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>351</v>
       </c>
@@ -9199,7 +9197,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>351</v>
       </c>
@@ -9228,7 +9226,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>351</v>
       </c>
@@ -9257,7 +9255,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>351</v>
       </c>
@@ -9286,7 +9284,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>351</v>
       </c>
@@ -9315,7 +9313,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>351</v>
       </c>
@@ -9344,7 +9342,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>351</v>
       </c>
@@ -9373,7 +9371,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>351</v>
       </c>
@@ -9402,7 +9400,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>351</v>
       </c>
@@ -9431,7 +9429,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>351</v>
       </c>
@@ -9460,7 +9458,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>351</v>
       </c>
@@ -9489,7 +9487,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>351</v>
       </c>
@@ -9518,7 +9516,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>351</v>
       </c>
@@ -9547,7 +9545,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>351</v>
       </c>
@@ -9576,7 +9574,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>351</v>
       </c>
@@ -9605,7 +9603,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>351</v>
       </c>
@@ -9637,7 +9635,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>351</v>
       </c>
@@ -9666,7 +9664,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>351</v>
       </c>
@@ -9695,7 +9693,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>351</v>
       </c>
@@ -9724,7 +9722,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>351</v>
       </c>
@@ -9753,7 +9751,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>351</v>
       </c>
@@ -9782,7 +9780,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>351</v>
       </c>
@@ -9811,7 +9809,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>351</v>
       </c>
@@ -9840,7 +9838,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>351</v>
       </c>
@@ -9869,7 +9867,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>351</v>
       </c>
@@ -9898,7 +9896,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>351</v>
       </c>
@@ -9927,7 +9925,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>351</v>
       </c>
@@ -9956,7 +9954,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>351</v>
       </c>
@@ -9985,7 +9983,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>351</v>
       </c>
@@ -10014,7 +10012,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>351</v>
       </c>
@@ -10043,7 +10041,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>351</v>
       </c>
@@ -10072,7 +10070,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156" s="3" t="s">
         <v>351</v>
       </c>
@@ -10101,7 +10099,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>351</v>
       </c>
@@ -10130,7 +10128,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>351</v>
       </c>
@@ -10159,7 +10157,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>477</v>
       </c>
@@ -10167,7 +10165,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160" s="7"/>
       <c r="B160" s="14"/>
       <c r="C160" s="7"/>
@@ -10180,12 +10178,12 @@
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B161" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -10198,12 +10196,12 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B163" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -10216,12 +10214,12 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B165" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -10234,12 +10232,12 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B167" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -10252,12 +10250,12 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B169" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -10270,12 +10268,12 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B171" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -10288,7 +10286,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B173" s="3" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
Corrected error in spreadsheet
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D8E06-0389-41B8-9B42-012C975F454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D412B193-70DB-41C7-969A-775F2A9ECCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_precision_recall" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="584">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1790,7 +1792,16 @@
     <t xml:space="preserve"> (discard in the likely case it is very innacurate) </t>
   </si>
   <si>
-    <t>(re-do once Axel is done wiht the new function)</t>
+    <t>"advtime_position_005a"</t>
+  </si>
+  <si>
+    <t>"advtime_durfreq_005b"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time adverbials on location in time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time adverbials on frequency or duration</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1947,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2033,7 +2044,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2336,14 +2347,14 @@
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.796875" customWidth="1"/>
-    <col min="2" max="2" width="32.46484375" customWidth="1"/>
-    <col min="3" max="3" width="23.265625" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2374,7 +2385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2388,7 +2399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2416,7 +2427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2430,7 +2441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2444,7 +2455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2456,7 +2467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2468,7 +2479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2480,7 +2491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -2492,7 +2503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2504,7 +2515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
@@ -2515,7 +2526,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2529,7 +2540,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2543,7 +2554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2555,7 +2566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -2569,7 +2580,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2581,7 +2592,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2595,7 +2606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -2609,7 +2620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -2623,7 +2634,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2637,7 +2648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -2649,7 +2660,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2661,7 +2672,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -2675,7 +2686,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -2689,7 +2700,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2703,7 +2714,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2717,7 +2728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2731,7 +2742,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2745,7 +2756,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2757,7 +2768,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2769,7 +2780,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -2781,7 +2792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>102</v>
       </c>
@@ -2793,7 +2804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2807,7 +2818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>107</v>
       </c>
@@ -2819,7 +2830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2831,7 +2842,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -2843,7 +2854,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -2853,7 +2864,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -2865,7 +2876,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2877,7 +2888,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>122</v>
       </c>
@@ -2891,7 +2902,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -2905,7 +2916,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -2917,7 +2928,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>131</v>
       </c>
@@ -2927,7 +2938,7 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>133</v>
       </c>
@@ -2937,7 +2948,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2951,7 +2962,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
@@ -2965,7 +2976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>141</v>
       </c>
@@ -2975,7 +2986,7 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>143</v>
       </c>
@@ -2989,7 +3000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>145</v>
       </c>
@@ -3006,7 +3017,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -3020,7 +3031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -3034,7 +3045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
@@ -3048,7 +3059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>155</v>
       </c>
@@ -3062,7 +3073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>158</v>
       </c>
@@ -3074,7 +3085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>160</v>
       </c>
@@ -3088,7 +3099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -3102,7 +3113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
@@ -3116,7 +3127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>166</v>
       </c>
@@ -3128,7 +3139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
@@ -3142,7 +3153,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -3156,7 +3167,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>176</v>
       </c>
@@ -3168,7 +3179,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
@@ -3182,7 +3193,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>182</v>
       </c>
@@ -3196,7 +3207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>184</v>
       </c>
@@ -3208,7 +3219,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>186</v>
       </c>
@@ -3220,7 +3231,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3232,7 +3243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3244,7 +3255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
@@ -3254,7 +3265,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>195</v>
       </c>
@@ -3264,7 +3275,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
@@ -3274,7 +3285,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3284,7 +3295,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>201</v>
       </c>
@@ -3298,7 +3309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>543</v>
       </c>
@@ -3308,7 +3319,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>541</v>
       </c>
@@ -3318,7 +3329,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>204</v>
       </c>
@@ -3330,7 +3341,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>206</v>
       </c>
@@ -3342,7 +3353,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
@@ -3354,7 +3365,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>210</v>
       </c>
@@ -3366,7 +3377,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>439</v>
       </c>
@@ -3378,7 +3389,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>440</v>
       </c>
@@ -3390,7 +3401,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>442</v>
       </c>
@@ -3401,7 +3412,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>441</v>
       </c>
@@ -3412,7 +3423,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>545</v>
       </c>
@@ -3423,7 +3434,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>547</v>
       </c>
@@ -3434,7 +3445,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>549</v>
       </c>
@@ -3453,25 +3464,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7223C10B-8642-4163-B1BD-0866630178C4}">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.265625" customWidth="1"/>
-    <col min="2" max="2" width="22.73046875" customWidth="1"/>
-    <col min="3" max="4" width="7.265625" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="4" width="7.26953125" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3503,7 +3514,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3526,7 +3537,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3549,7 +3560,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3561,19 +3572,19 @@
       </c>
       <c r="D4" s="21"/>
       <c r="I4" t="e">
-        <f t="shared" ref="I4:I8" si="0">E4/(E4+G4)</f>
+        <f t="shared" ref="I4:I9" si="0">E4/(E4+G4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J4" t="e">
-        <f t="shared" ref="J4:J8" si="1">E4/(E4+H4)</f>
+        <f t="shared" ref="J4:J9" si="1">E4/(E4+H4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K4" t="e">
-        <f t="shared" ref="K4:K8" si="2">2*((I4*J4)/(I4+J4))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="K4:K9" si="2">2*((I4*J4)/(I4+J4))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3596,7 +3607,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -3619,40 +3630,28 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>580</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>580</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="I7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+        <v>582</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>581</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>539</v>
-      </c>
+        <v>583</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" s="21"/>
       <c r="I8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3666,58 +3665,58 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>539</v>
       </c>
       <c r="I9" t="e">
-        <f t="shared" ref="I9:I70" si="3">E9/(E9+G9)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J9" t="e">
-        <f t="shared" ref="J9:J70" si="4">E9/(E9+H9)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K9" t="e">
-        <f t="shared" ref="K9:K70" si="5">2*((I9*J9)/(I9+J9))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>539</v>
       </c>
       <c r="I10" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I10:I71" si="3">E10/(E10+G10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J10:J71" si="4">E10/(E10+H10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="K10:K71" si="5">2*((I10*J10)/(I10+J10))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>539</v>
@@ -3735,17 +3734,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>574</v>
-      </c>
-      <c r="D12" s="21"/>
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>539</v>
+      </c>
       <c r="I12" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3759,16 +3757,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>539</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="D13" s="21"/>
       <c r="I13" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3782,12 +3781,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>539</v>
@@ -3805,17 +3804,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>560</v>
-      </c>
-      <c r="D15" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>539</v>
+      </c>
       <c r="I15" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3829,16 +3827,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>560</v>
       </c>
+      <c r="D16" s="11"/>
       <c r="I16" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3852,17 +3851,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D17" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>560</v>
+      </c>
       <c r="I17" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3876,12 +3874,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>539</v>
@@ -3900,17 +3898,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D19" s="11"/>
       <c r="I19" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3924,19 +3922,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>575</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D20" s="21"/>
       <c r="I20" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -3950,15 +3946,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>539</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>575</v>
       </c>
       <c r="I21" t="e">
         <f t="shared" si="3"/>
@@ -3973,12 +3972,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
         <v>539</v>
@@ -3996,17 +3995,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
         <v>539</v>
       </c>
-      <c r="D23" s="11"/>
       <c r="I23" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4020,19 +4018,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>577</v>
-      </c>
+      <c r="D24" s="11"/>
       <c r="I24" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4046,17 +4042,19 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D25" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>577</v>
+      </c>
       <c r="I25" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4070,17 +4068,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D26" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D26" s="21"/>
       <c r="I26" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4094,17 +4092,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="11"/>
       <c r="I27" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4118,19 +4116,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>576</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>577</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D28" s="21"/>
       <c r="I28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4144,12 +4140,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>576</v>
@@ -4170,15 +4166,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>577</v>
@@ -4196,17 +4192,19 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D31" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>578</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>577</v>
+      </c>
       <c r="I31" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4220,12 +4218,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>539</v>
@@ -4244,17 +4242,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>570</v>
-      </c>
-      <c r="D33" s="20"/>
+        <v>99</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D33" s="11"/>
       <c r="I33" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4268,12 +4266,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>570</v>
@@ -4292,17 +4290,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D35" s="21"/>
+        <v>103</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>570</v>
+      </c>
+      <c r="D35" s="20"/>
       <c r="I35" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4316,19 +4314,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>579</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D36" s="21"/>
       <c r="I36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4342,17 +4338,19 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="22" t="s">
+        <v>579</v>
+      </c>
       <c r="I37" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4366,17 +4364,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="2"/>
       <c r="I38" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4390,12 +4388,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>539</v>
@@ -4414,12 +4412,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>539</v>
@@ -4438,16 +4436,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>539</v>
       </c>
+      <c r="D41" s="11"/>
       <c r="I41" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4461,12 +4460,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
         <v>539</v>
@@ -4484,12 +4483,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
         <v>539</v>
@@ -4507,17 +4506,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D44" s="21"/>
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>539</v>
+      </c>
       <c r="I44" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4531,17 +4529,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D45" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D45" s="21"/>
       <c r="I45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4555,17 +4553,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D46" s="21"/>
+        <v>571</v>
+      </c>
+      <c r="D46" s="11"/>
       <c r="I46" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4579,17 +4577,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D47" s="11"/>
+      <c r="D47" s="21"/>
       <c r="I47" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4603,12 +4601,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>539</v>
@@ -4627,17 +4625,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D49" s="21"/>
+        <v>142</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D49" s="11"/>
       <c r="I49" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4651,17 +4649,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="D50" s="11"/>
+        <v>565</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="D50" s="21"/>
       <c r="I50" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4675,17 +4673,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>574</v>
-      </c>
-      <c r="D51" s="21"/>
+        <v>148</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D51" s="11"/>
       <c r="I51" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4699,16 +4697,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" t="s">
-        <v>539</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="D52" s="21"/>
       <c r="I52" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4722,17 +4721,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" t="s">
         <v>539</v>
       </c>
-      <c r="D53" s="11"/>
       <c r="I53" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4746,16 +4744,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>539</v>
       </c>
+      <c r="D54" s="11"/>
       <c r="I54" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4769,12 +4768,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
         <v>539</v>
@@ -4792,12 +4791,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C56" t="s">
         <v>539</v>
@@ -4815,12 +4814,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
         <v>539</v>
@@ -4838,12 +4837,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
         <v>539</v>
@@ -4861,12 +4860,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C59" t="s">
         <v>539</v>
@@ -4884,17 +4883,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C60" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" t="s">
         <v>539</v>
       </c>
-      <c r="D60" s="11"/>
       <c r="I60" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4908,12 +4906,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>539</v>
@@ -4932,12 +4930,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>539</v>
@@ -4956,12 +4954,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>539</v>
@@ -4980,12 +4978,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>539</v>
@@ -5004,12 +5002,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>539</v>
@@ -5028,12 +5026,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>539</v>
@@ -5052,12 +5050,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>539</v>
@@ -5076,16 +5074,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C68" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>539</v>
       </c>
+      <c r="D68" s="11"/>
       <c r="I68" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -5099,12 +5098,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C69" t="s">
         <v>539</v>
@@ -5122,17 +5121,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C70" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" t="s">
         <v>539</v>
       </c>
-      <c r="D70" s="11"/>
       <c r="I70" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -5146,60 +5144,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>539</v>
       </c>
       <c r="D71" s="11"/>
       <c r="I71" t="e">
-        <f t="shared" ref="I71:I80" si="6">E71/(E71+G71)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J71" t="e">
-        <f t="shared" ref="J71:J80" si="7">E71/(E71+H71)</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K71" t="e">
-        <f t="shared" ref="K71:K80" si="8">2*((I71*J71)/(I71+J71))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>539</v>
       </c>
       <c r="D72" s="11"/>
       <c r="I72" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="I72:I81" si="6">E72/(E72+G72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J72" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J72:J81" si="7">E72/(E72+H72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K72" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="K72:K81" si="8">2*((I72*J72)/(I72+J72))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>543</v>
+        <v>201</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>542</v>
+        <v>202</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>539</v>
@@ -5218,12 +5216,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>539</v>
@@ -5242,16 +5240,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>204</v>
+        <v>541</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C75" t="s">
+        <v>540</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>539</v>
       </c>
+      <c r="D75" s="11"/>
       <c r="I75" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5265,12 +5264,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C76" t="s">
         <v>539</v>
@@ -5288,17 +5287,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>573</v>
-      </c>
-      <c r="D77" s="11"/>
+        <v>207</v>
+      </c>
+      <c r="C77" t="s">
+        <v>539</v>
+      </c>
       <c r="I77" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -5312,12 +5310,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>573</v>
@@ -5336,15 +5334,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>439</v>
+        <v>210</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>443</v>
+        <v>211</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>539</v>
+        <v>573</v>
       </c>
       <c r="D79" s="11"/>
       <c r="I79" t="e">
@@ -5360,12 +5358,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>539</v>
@@ -5384,65 +5382,89 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>568</v>
-      </c>
-      <c r="B81" t="s">
-        <v>445</v>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>444</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>539</v>
       </c>
       <c r="D81" s="11"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="I81" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J81" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K81" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>539</v>
       </c>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>569</v>
+      </c>
+      <c r="B83" t="s">
+        <v>446</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D83" s="11"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>545</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>544</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C84" s="21" t="s">
         <v>567</v>
       </c>
-      <c r="D83" s="21"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+      <c r="D84" s="21"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>547</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>546</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C85" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="D84" s="11"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>549</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>548</v>
       </c>
-      <c r="C85" s="21" t="s">
+      <c r="C86" s="21" t="s">
         <v>567</v>
       </c>
-      <c r="D85" s="21"/>
+      <c r="D86" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5459,22 +5481,22 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.53125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" style="3"/>
+    <col min="1" max="1" width="9.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="3"/>
     <col min="4" max="4" width="9" style="4" customWidth="1"/>
     <col min="5" max="5" width="55" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.46484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="3" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
     <col min="8" max="8" width="8" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.265625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
@@ -5509,7 +5531,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>221</v>
       </c>
@@ -5538,7 +5560,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>221</v>
       </c>
@@ -5567,7 +5589,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>221</v>
       </c>
@@ -5596,7 +5618,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>221</v>
       </c>
@@ -5625,7 +5647,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>221</v>
       </c>
@@ -5654,7 +5676,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -5683,7 +5705,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>221</v>
       </c>
@@ -5715,7 +5737,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>221</v>
       </c>
@@ -5747,7 +5769,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>221</v>
       </c>
@@ -5779,7 +5801,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>221</v>
       </c>
@@ -5808,7 +5830,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>221</v>
       </c>
@@ -5840,7 +5862,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>221</v>
       </c>
@@ -5872,7 +5894,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>221</v>
       </c>
@@ -5901,7 +5923,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>221</v>
       </c>
@@ -5930,7 +5952,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>221</v>
       </c>
@@ -5962,7 +5984,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>221</v>
       </c>
@@ -5993,7 +6015,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>221</v>
       </c>
@@ -6026,7 +6048,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>221</v>
       </c>
@@ -6056,7 +6078,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>221</v>
       </c>
@@ -6085,7 +6107,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>221</v>
       </c>
@@ -6114,7 +6136,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>221</v>
       </c>
@@ -6146,7 +6168,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>221</v>
       </c>
@@ -6175,7 +6197,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>221</v>
       </c>
@@ -6204,7 +6226,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>221</v>
       </c>
@@ -6233,7 +6255,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>221</v>
       </c>
@@ -6262,7 +6284,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>221</v>
       </c>
@@ -6291,7 +6313,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>221</v>
       </c>
@@ -6320,7 +6342,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>221</v>
       </c>
@@ -6349,7 +6371,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -6381,7 +6403,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>221</v>
       </c>
@@ -6410,7 +6432,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>221</v>
       </c>
@@ -6439,7 +6461,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>221</v>
       </c>
@@ -6468,7 +6490,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>221</v>
       </c>
@@ -6497,7 +6519,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>221</v>
       </c>
@@ -6526,7 +6548,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>221</v>
       </c>
@@ -6558,7 +6580,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>221</v>
       </c>
@@ -6590,7 +6612,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>221</v>
       </c>
@@ -6622,7 +6644,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>221</v>
       </c>
@@ -6654,7 +6676,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>221</v>
       </c>
@@ -6683,7 +6705,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>221</v>
       </c>
@@ -6712,7 +6734,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>221</v>
       </c>
@@ -6741,7 +6763,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>221</v>
       </c>
@@ -6770,7 +6792,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>221</v>
       </c>
@@ -6802,7 +6824,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>221</v>
       </c>
@@ -6831,7 +6853,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>221</v>
       </c>
@@ -6860,7 +6882,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>221</v>
       </c>
@@ -6889,7 +6911,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>257</v>
       </c>
@@ -6918,7 +6940,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>257</v>
       </c>
@@ -6947,7 +6969,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>257</v>
       </c>
@@ -6976,7 +6998,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>257</v>
       </c>
@@ -7005,7 +7027,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>257</v>
       </c>
@@ -7034,7 +7056,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>257</v>
       </c>
@@ -7063,7 +7085,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>257</v>
       </c>
@@ -7092,7 +7114,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>257</v>
       </c>
@@ -7121,7 +7143,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>257</v>
       </c>
@@ -7150,7 +7172,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>257</v>
       </c>
@@ -7179,7 +7201,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>257</v>
       </c>
@@ -7208,7 +7230,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>257</v>
       </c>
@@ -7239,7 +7261,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>257</v>
       </c>
@@ -7270,7 +7292,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>257</v>
       </c>
@@ -7299,7 +7321,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>257</v>
       </c>
@@ -7328,7 +7350,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>257</v>
       </c>
@@ -7357,7 +7379,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>257</v>
       </c>
@@ -7386,7 +7408,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>257</v>
       </c>
@@ -7415,7 +7437,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>257</v>
       </c>
@@ -7444,7 +7466,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>257</v>
       </c>
@@ -7473,7 +7495,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>257</v>
       </c>
@@ -7502,7 +7524,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>257</v>
       </c>
@@ -7531,7 +7553,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>257</v>
       </c>
@@ -7560,7 +7582,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>257</v>
       </c>
@@ -7589,7 +7611,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
@@ -7618,7 +7640,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>257</v>
       </c>
@@ -7647,7 +7669,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>257</v>
       </c>
@@ -7676,7 +7698,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>257</v>
       </c>
@@ -7705,7 +7727,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>257</v>
       </c>
@@ -7734,7 +7756,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>257</v>
       </c>
@@ -7763,7 +7785,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>257</v>
       </c>
@@ -7792,7 +7814,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>257</v>
       </c>
@@ -7821,7 +7843,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>257</v>
       </c>
@@ -7850,7 +7872,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>257</v>
       </c>
@@ -7879,7 +7901,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>257</v>
       </c>
@@ -7908,7 +7930,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>257</v>
       </c>
@@ -7937,7 +7959,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>257</v>
       </c>
@@ -7969,7 +7991,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>257</v>
       </c>
@@ -8001,7 +8023,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -8030,7 +8052,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>257</v>
       </c>
@@ -8062,7 +8084,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>257</v>
       </c>
@@ -8094,7 +8116,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>257</v>
       </c>
@@ -8129,7 +8151,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>257</v>
       </c>
@@ -8161,7 +8183,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>257</v>
       </c>
@@ -8193,7 +8215,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>257</v>
       </c>
@@ -8222,7 +8244,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>257</v>
       </c>
@@ -8251,7 +8273,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>257</v>
       </c>
@@ -8280,7 +8302,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>257</v>
       </c>
@@ -8309,7 +8331,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>257</v>
       </c>
@@ -8338,7 +8360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>257</v>
       </c>
@@ -8367,7 +8389,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>257</v>
       </c>
@@ -8396,7 +8418,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>257</v>
       </c>
@@ -8425,7 +8447,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>257</v>
       </c>
@@ -8457,7 +8479,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>257</v>
       </c>
@@ -8486,7 +8508,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>257</v>
       </c>
@@ -8515,7 +8537,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>257</v>
       </c>
@@ -8546,7 +8568,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="9"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>257</v>
       </c>
@@ -8576,7 +8598,7 @@
       </c>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>257</v>
       </c>
@@ -8607,7 +8629,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="9"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>257</v>
       </c>
@@ -8638,7 +8660,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="9"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>257</v>
       </c>
@@ -8669,7 +8691,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="9"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>257</v>
       </c>
@@ -8700,7 +8722,7 @@
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
@@ -8731,7 +8753,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>257</v>
       </c>
@@ -8762,7 +8784,7 @@
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>257</v>
       </c>
@@ -8791,7 +8813,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>257</v>
       </c>
@@ -8820,7 +8842,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>257</v>
       </c>
@@ -8849,7 +8871,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>351</v>
       </c>
@@ -8878,7 +8900,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>351</v>
       </c>
@@ -8907,7 +8929,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>351</v>
       </c>
@@ -8936,7 +8958,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>351</v>
       </c>
@@ -8965,7 +8987,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>351</v>
       </c>
@@ -8994,7 +9016,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>351</v>
       </c>
@@ -9023,7 +9045,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>351</v>
       </c>
@@ -9052,7 +9074,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>351</v>
       </c>
@@ -9081,7 +9103,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>351</v>
       </c>
@@ -9110,7 +9132,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>351</v>
       </c>
@@ -9139,7 +9161,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>351</v>
       </c>
@@ -9168,7 +9190,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>351</v>
       </c>
@@ -9197,7 +9219,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>351</v>
       </c>
@@ -9226,7 +9248,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>351</v>
       </c>
@@ -9255,7 +9277,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>351</v>
       </c>
@@ -9284,7 +9306,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>351</v>
       </c>
@@ -9313,7 +9335,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>351</v>
       </c>
@@ -9342,7 +9364,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>351</v>
       </c>
@@ -9371,7 +9393,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>351</v>
       </c>
@@ -9400,7 +9422,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>351</v>
       </c>
@@ -9429,7 +9451,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>351</v>
       </c>
@@ -9458,7 +9480,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>351</v>
       </c>
@@ -9487,7 +9509,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>351</v>
       </c>
@@ -9516,7 +9538,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>351</v>
       </c>
@@ -9545,7 +9567,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>351</v>
       </c>
@@ -9574,7 +9596,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>351</v>
       </c>
@@ -9603,7 +9625,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>351</v>
       </c>
@@ -9635,7 +9657,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>351</v>
       </c>
@@ -9664,7 +9686,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>351</v>
       </c>
@@ -9693,7 +9715,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>351</v>
       </c>
@@ -9722,7 +9744,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>351</v>
       </c>
@@ -9751,7 +9773,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>351</v>
       </c>
@@ -9780,7 +9802,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>351</v>
       </c>
@@ -9809,7 +9831,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>351</v>
       </c>
@@ -9838,7 +9860,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>351</v>
       </c>
@@ -9867,7 +9889,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>351</v>
       </c>
@@ -9896,7 +9918,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>351</v>
       </c>
@@ -9925,7 +9947,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>351</v>
       </c>
@@ -9954,7 +9976,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>351</v>
       </c>
@@ -9983,7 +10005,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
         <v>351</v>
       </c>
@@ -10012,7 +10034,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>351</v>
       </c>
@@ -10041,7 +10063,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
         <v>351</v>
       </c>
@@ -10070,7 +10092,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
         <v>351</v>
       </c>
@@ -10099,7 +10121,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="s">
         <v>351</v>
       </c>
@@ -10128,7 +10150,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
         <v>351</v>
       </c>
@@ -10157,7 +10179,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
         <v>477</v>
       </c>
@@ -10165,7 +10187,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" s="7"/>
       <c r="B160" s="14"/>
       <c r="C160" s="7"/>
@@ -10178,12 +10200,12 @@
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B161" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -10196,12 +10218,12 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B163" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -10214,12 +10236,12 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B165" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -10232,12 +10254,12 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B167" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -10250,12 +10272,12 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B169" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -10268,12 +10290,12 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B171" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -10286,7 +10308,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B173" s="3" t="s">
         <v>484</v>
       </c>

</xml_diff>

<commit_message>
Continued manual feature coding, corrected script, added some new items for reddit_vocab
</commit_message>
<xml_diff>
--- a/Overview_feature_extraction_precision_recall.xlsx
+++ b/Overview_feature_extraction_precision_recall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D412B193-70DB-41C7-969A-775F2A9ECCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1196B490-BB86-4E8E-9181-771D74FDE261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="586">
   <si>
     <t>Feature_name</t>
   </si>
@@ -1802,6 +1802,12 @@
   </si>
   <si>
     <t xml:space="preserve"> time adverbials on frequency or duration</t>
+  </si>
+  <si>
+    <t>good to go (Axel)</t>
+  </si>
+  <si>
+    <t>(feel very unsure whether I did this correctly)</t>
   </si>
 </sst>
 </file>
@@ -3468,7 +3474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3637,8 +3643,8 @@
       <c r="B7" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>567</v>
+      <c r="C7" s="11" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3648,8 +3654,8 @@
       <c r="B8" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>567</v>
+      <c r="C8" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="D8" s="21"/>
       <c r="I8" t="e">
@@ -3930,7 +3936,7 @@
         <v>58</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="D20" s="21"/>
       <c r="I20" t="e">
@@ -4147,8 +4153,8 @@
       <c r="B29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="21" t="s">
-        <v>576</v>
+      <c r="C29" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>577</v>
@@ -4536,10 +4542,12 @@
       <c r="B45" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D45" s="21"/>
+      <c r="C45" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>585</v>
+      </c>
       <c r="I45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -4656,8 +4664,8 @@
       <c r="B50" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>567</v>
+      <c r="C50" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="D50" s="21"/>
       <c r="I50" t="e">
@@ -5437,8 +5445,8 @@
       <c r="B84" t="s">
         <v>544</v>
       </c>
-      <c r="C84" s="21" t="s">
-        <v>567</v>
+      <c r="C84" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="D84" s="21"/>
     </row>
@@ -5461,8 +5469,8 @@
       <c r="B86" t="s">
         <v>548</v>
       </c>
-      <c r="C86" s="21" t="s">
-        <v>567</v>
+      <c r="C86" s="11" t="s">
+        <v>573</v>
       </c>
       <c r="D86" s="21"/>
     </row>

</xml_diff>